<commit_message>
[Presentazione] Aggiornata presentazione + pdf
</commit_message>
<xml_diff>
--- a/RP/Esterni/Piano di Progetto/Ripartizione ruoli e ore.xlsx
+++ b/RP/Esterni/Piano di Progetto/Ripartizione ruoli e ore.xlsx
@@ -1530,45 +1530,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1583,28 +1548,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1614,6 +1605,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2039,12 +2039,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="98229248"/>
-        <c:axId val="98231040"/>
+        <c:axId val="66619264"/>
+        <c:axId val="66620800"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="98229248"/>
+        <c:axId val="66619264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2053,7 +2053,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98231040"/>
+        <c:crossAx val="66620800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2061,7 +2061,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98231040"/>
+        <c:axId val="66620800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2072,7 +2072,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98229248"/>
+        <c:crossAx val="66619264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2262,12 +2262,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="101029376"/>
-        <c:axId val="101030912"/>
+        <c:axId val="75310208"/>
+        <c:axId val="75311744"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="101029376"/>
+        <c:axId val="75310208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2276,7 +2276,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101030912"/>
+        <c:crossAx val="75311744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2284,7 +2284,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101030912"/>
+        <c:axId val="75311744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2295,9 +2295,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101029376"/>
+        <c:crossAx val="75310208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="100"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2830,11 +2831,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="102923648"/>
-        <c:axId val="102937728"/>
+        <c:axId val="76295168"/>
+        <c:axId val="76313344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102923648"/>
+        <c:axId val="76295168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2843,7 +2844,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102937728"/>
+        <c:crossAx val="76313344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2851,7 +2852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102937728"/>
+        <c:axId val="76313344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2862,7 +2863,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102923648"/>
+        <c:crossAx val="76295168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3677,19 +3678,19 @@
         <f>'1_AN'!O2</f>
         <v>Membro</v>
       </c>
-      <c r="AC2" s="185" t="str">
+      <c r="AC2" s="189" t="str">
         <f>'1_AN'!P2</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD2" s="186"/>
-      <c r="AE2" s="187"/>
-      <c r="AF2" s="185" t="str">
+      <c r="AD2" s="190"/>
+      <c r="AE2" s="191"/>
+      <c r="AF2" s="189" t="str">
         <f>'1_AN'!S2</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG2" s="186"/>
-      <c r="AH2" s="186"/>
-      <c r="AI2" s="188" t="str">
+      <c r="AG2" s="190"/>
+      <c r="AH2" s="190"/>
+      <c r="AI2" s="183" t="str">
         <f>'1_AN'!V2</f>
         <v>Totale</v>
       </c>
@@ -3823,7 +3824,7 @@
         <f>'1_AN'!U3</f>
         <v>Fase</v>
       </c>
-      <c r="AI3" s="189"/>
+      <c r="AI3" s="184"/>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="147" t="s">
@@ -4706,25 +4707,25 @@
       <c r="AB12" s="149" t="s">
         <v>126</v>
       </c>
-      <c r="AC12" s="185" t="str">
+      <c r="AC12" s="189" t="str">
         <f>'2_PA'!V9</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD12" s="190"/>
-      <c r="AE12" s="191"/>
-      <c r="AF12" s="192" t="str">
+      <c r="AD12" s="192"/>
+      <c r="AE12" s="193"/>
+      <c r="AF12" s="179" t="str">
         <f>'2_PA'!Y9</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG12" s="193"/>
-      <c r="AH12" s="194"/>
-      <c r="AI12" s="192" t="str">
+      <c r="AG12" s="180"/>
+      <c r="AH12" s="181"/>
+      <c r="AI12" s="179" t="str">
         <f>'2_PA'!AB9</f>
         <v>III Periodo</v>
       </c>
-      <c r="AJ12" s="193"/>
-      <c r="AK12" s="195"/>
-      <c r="AL12" s="188" t="str">
+      <c r="AJ12" s="180"/>
+      <c r="AK12" s="182"/>
+      <c r="AL12" s="183" t="str">
         <f>'2_PA'!AE9</f>
         <v>Totale</v>
       </c>
@@ -4775,7 +4776,7 @@
         <f>'2_PA'!AD10</f>
         <v>Fase</v>
       </c>
-      <c r="AL13" s="189"/>
+      <c r="AL13" s="184"/>
       <c r="AM13">
         <f>SUM(AL14:AL27)</f>
         <v>193</v>
@@ -4830,7 +4831,7 @@
         <f>'2_PA'!AD11</f>
         <v>PA 3.2</v>
       </c>
-      <c r="AL14" s="196">
+      <c r="AL14" s="185">
         <f>'2_PA'!AE11</f>
         <v>26</v>
       </c>
@@ -4960,7 +4961,7 @@
         <f>'2_PA'!AD12</f>
         <v>0</v>
       </c>
-      <c r="AL15" s="184"/>
+      <c r="AL15" s="177"/>
       <c r="AO15">
         <f>IF($AC15=AO$2,$AD15,0)</f>
         <v>0</v>
@@ -5079,7 +5080,7 @@
         <f>'2_PA'!AD13</f>
         <v>PA 3.2</v>
       </c>
-      <c r="AL16" s="184">
+      <c r="AL16" s="177">
         <f>'2_PA'!AE13</f>
         <v>27</v>
       </c>
@@ -5201,7 +5202,7 @@
         <f>'2_PA'!AD14</f>
         <v>0</v>
       </c>
-      <c r="AL17" s="184"/>
+      <c r="AL17" s="177"/>
       <c r="AO17">
         <f t="shared" si="35"/>
         <v>0</v>
@@ -5320,7 +5321,7 @@
         <f>'2_PA'!AD15</f>
         <v>PA 3.3</v>
       </c>
-      <c r="AL18" s="184">
+      <c r="AL18" s="177">
         <f>'2_PA'!AE15</f>
         <v>26</v>
       </c>
@@ -5442,7 +5443,7 @@
         <f>'2_PA'!AD16</f>
         <v>PA 6.1</v>
       </c>
-      <c r="AL19" s="184"/>
+      <c r="AL19" s="177"/>
       <c r="AO19">
         <f t="shared" si="35"/>
         <v>0</v>
@@ -5561,7 +5562,7 @@
         <f>'2_PA'!AD17</f>
         <v>PA 3.3</v>
       </c>
-      <c r="AL20" s="184">
+      <c r="AL20" s="177">
         <f>'2_PA'!AE17</f>
         <v>28</v>
       </c>
@@ -5683,7 +5684,7 @@
         <f>'2_PA'!AD18</f>
         <v>PA 6.2</v>
       </c>
-      <c r="AL21" s="184"/>
+      <c r="AL21" s="177"/>
       <c r="AO21">
         <f t="shared" si="35"/>
         <v>0</v>
@@ -5802,7 +5803,7 @@
         <f>'2_PA'!AD19</f>
         <v>PA 5.1</v>
       </c>
-      <c r="AL22" s="184">
+      <c r="AL22" s="177">
         <f>'2_PA'!AE19</f>
         <v>30</v>
       </c>
@@ -5887,36 +5888,36 @@
       <c r="A23" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="197" t="s">
+      <c r="B23" s="194" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="197"/>
-      <c r="D23" s="197"/>
-      <c r="E23" s="197" t="s">
+      <c r="C23" s="194"/>
+      <c r="D23" s="194"/>
+      <c r="E23" s="194" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="197"/>
-      <c r="G23" s="197"/>
-      <c r="H23" s="197" t="s">
+      <c r="F23" s="194"/>
+      <c r="G23" s="194"/>
+      <c r="H23" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="I23" s="197"/>
-      <c r="J23" s="197"/>
-      <c r="K23" s="197" t="s">
+      <c r="I23" s="194"/>
+      <c r="J23" s="194"/>
+      <c r="K23" s="194" t="s">
         <v>4</v>
       </c>
-      <c r="L23" s="197"/>
-      <c r="M23" s="197"/>
-      <c r="N23" s="197" t="s">
+      <c r="L23" s="194"/>
+      <c r="M23" s="194"/>
+      <c r="N23" s="194" t="s">
         <v>5</v>
       </c>
-      <c r="O23" s="197"/>
-      <c r="P23" s="197"/>
-      <c r="Q23" s="197" t="s">
+      <c r="O23" s="194"/>
+      <c r="P23" s="194"/>
+      <c r="Q23" s="194" t="s">
         <v>6</v>
       </c>
-      <c r="R23" s="197"/>
-      <c r="S23" s="197"/>
+      <c r="R23" s="194"/>
+      <c r="S23" s="194"/>
       <c r="T23" s="159" t="s">
         <v>14</v>
       </c>
@@ -5961,7 +5962,7 @@
         <f>'2_PA'!AD20</f>
         <v>0</v>
       </c>
-      <c r="AL23" s="184"/>
+      <c r="AL23" s="177"/>
       <c r="AO23">
         <f t="shared" si="35"/>
         <v>0</v>
@@ -6040,50 +6041,50 @@
       </c>
     </row>
     <row r="24" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A24" s="183" t="s">
+      <c r="A24" s="186" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="181">
+      <c r="B24" s="188">
         <f>SUM(AO4:AQ4,AO14:AQ15,AO31:AQ32,AO48:AQ49)</f>
         <v>17</v>
       </c>
-      <c r="C24" s="181"/>
-      <c r="D24" s="181"/>
-      <c r="E24" s="181">
+      <c r="C24" s="188"/>
+      <c r="D24" s="188"/>
+      <c r="E24" s="188">
         <f>SUM(AR4:AT4,AR14:AT15,AR31:AT32,AR48:AT49)</f>
         <v>10</v>
       </c>
-      <c r="F24" s="181"/>
-      <c r="G24" s="181"/>
-      <c r="H24" s="182">
+      <c r="F24" s="188"/>
+      <c r="G24" s="188"/>
+      <c r="H24" s="187">
         <f>SUM(AU4:AW4,AU14:AW15,AU31:AW32,AU48:AW49)</f>
         <v>15</v>
       </c>
-      <c r="I24" s="182"/>
-      <c r="J24" s="182"/>
-      <c r="K24" s="181">
+      <c r="I24" s="187"/>
+      <c r="J24" s="187"/>
+      <c r="K24" s="188">
         <f>SUM(AX4:AZ4,AX14:AZ15,AX31:AZ32,AX48:AZ49)</f>
         <v>10</v>
       </c>
-      <c r="L24" s="181"/>
-      <c r="M24" s="181"/>
-      <c r="N24" s="182">
+      <c r="L24" s="188"/>
+      <c r="M24" s="188"/>
+      <c r="N24" s="187">
         <f>SUM(BA4:BC4,BA14:BC15,BA31:BC32,BA48:BC49)</f>
         <v>59</v>
       </c>
-      <c r="O24" s="182"/>
-      <c r="P24" s="182"/>
-      <c r="Q24" s="181">
+      <c r="O24" s="187"/>
+      <c r="P24" s="187"/>
+      <c r="Q24" s="188">
         <f t="shared" ref="Q24" si="38">SUM(BD4:BF4,BD14:BF15,BD31:BF32,BD48:BF49)</f>
         <v>4</v>
       </c>
-      <c r="R24" s="181"/>
-      <c r="S24" s="181"/>
-      <c r="T24" s="178">
+      <c r="R24" s="188"/>
+      <c r="S24" s="188"/>
+      <c r="T24" s="197">
         <f t="shared" ref="T24" si="39">SUM(B24:S25)</f>
         <v>115</v>
       </c>
-      <c r="U24" s="177"/>
+      <c r="U24" s="196"/>
       <c r="AB24" s="31" t="str">
         <f>'2_PA'!U21</f>
         <v>Quadrio Giacomo</v>
@@ -6124,7 +6125,7 @@
         <f>'2_PA'!AD21</f>
         <v>PA 5.1, 6.2</v>
       </c>
-      <c r="AL24" s="184">
+      <c r="AL24" s="177">
         <f>'2_PA'!AE21</f>
         <v>28</v>
       </c>
@@ -6206,27 +6207,27 @@
       </c>
     </row>
     <row r="25" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A25" s="183"/>
-      <c r="B25" s="181"/>
-      <c r="C25" s="181"/>
-      <c r="D25" s="181"/>
-      <c r="E25" s="181"/>
-      <c r="F25" s="181"/>
-      <c r="G25" s="181"/>
-      <c r="H25" s="182"/>
-      <c r="I25" s="182"/>
-      <c r="J25" s="182"/>
-      <c r="K25" s="181"/>
-      <c r="L25" s="181"/>
-      <c r="M25" s="181"/>
-      <c r="N25" s="182"/>
-      <c r="O25" s="182"/>
-      <c r="P25" s="182"/>
-      <c r="Q25" s="181"/>
-      <c r="R25" s="181"/>
-      <c r="S25" s="181"/>
-      <c r="T25" s="178"/>
-      <c r="U25" s="177"/>
+      <c r="A25" s="186"/>
+      <c r="B25" s="188"/>
+      <c r="C25" s="188"/>
+      <c r="D25" s="188"/>
+      <c r="E25" s="188"/>
+      <c r="F25" s="188"/>
+      <c r="G25" s="188"/>
+      <c r="H25" s="187"/>
+      <c r="I25" s="187"/>
+      <c r="J25" s="187"/>
+      <c r="K25" s="188"/>
+      <c r="L25" s="188"/>
+      <c r="M25" s="188"/>
+      <c r="N25" s="187"/>
+      <c r="O25" s="187"/>
+      <c r="P25" s="187"/>
+      <c r="Q25" s="188"/>
+      <c r="R25" s="188"/>
+      <c r="S25" s="188"/>
+      <c r="T25" s="197"/>
+      <c r="U25" s="196"/>
       <c r="AB25" s="31">
         <f>'2_PA'!U22</f>
         <v>0</v>
@@ -6267,7 +6268,7 @@
         <f>'2_PA'!AD22</f>
         <v>0</v>
       </c>
-      <c r="AL25" s="184"/>
+      <c r="AL25" s="177"/>
       <c r="AO25">
         <f t="shared" si="35"/>
         <v>0</v>
@@ -6346,50 +6347,50 @@
       </c>
     </row>
     <row r="26" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A26" s="183" t="s">
+      <c r="A26" s="186" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="181">
+      <c r="B26" s="188">
         <f>SUM(AO5:AQ5,AO16:AQ17,AO33:AQ34,AO50:AQ51)</f>
         <v>13</v>
       </c>
-      <c r="C26" s="181"/>
-      <c r="D26" s="181"/>
-      <c r="E26" s="181">
+      <c r="C26" s="188"/>
+      <c r="D26" s="188"/>
+      <c r="E26" s="188">
         <f>SUM(AR5:AT5,AR16:AT17,AR33:AT34,AR50:AT51)</f>
         <v>10</v>
       </c>
-      <c r="F26" s="181"/>
-      <c r="G26" s="181"/>
-      <c r="H26" s="181">
+      <c r="F26" s="188"/>
+      <c r="G26" s="188"/>
+      <c r="H26" s="188">
         <f>SUM(AU5:AW5,AU16:AW17,AU33:AW34,AU50:AW51)</f>
         <v>11</v>
       </c>
-      <c r="I26" s="181"/>
-      <c r="J26" s="181"/>
-      <c r="K26" s="182">
+      <c r="I26" s="188"/>
+      <c r="J26" s="188"/>
+      <c r="K26" s="187">
         <f>SUM(AX5:AZ5,AX16:AZ17,AX33:AZ34,AX50:AZ51)</f>
         <v>41</v>
       </c>
-      <c r="L26" s="182"/>
-      <c r="M26" s="182"/>
-      <c r="N26" s="181">
+      <c r="L26" s="187"/>
+      <c r="M26" s="187"/>
+      <c r="N26" s="188">
         <f>SUM(BA5:BC5,BA16:BC17,BA33:BC34,BA50:BC51)</f>
         <v>29</v>
       </c>
-      <c r="O26" s="181"/>
-      <c r="P26" s="181"/>
-      <c r="Q26" s="181">
+      <c r="O26" s="188"/>
+      <c r="P26" s="188"/>
+      <c r="Q26" s="188">
         <f>SUM(BD5:BF5,BD16:BF17,BD33:BF34,BD50:BF51)</f>
         <v>12</v>
       </c>
-      <c r="R26" s="181"/>
-      <c r="S26" s="181"/>
-      <c r="T26" s="178">
+      <c r="R26" s="188"/>
+      <c r="S26" s="188"/>
+      <c r="T26" s="197">
         <f t="shared" ref="T26" si="40">SUM(B26:S27)</f>
         <v>116</v>
       </c>
-      <c r="U26" s="177"/>
+      <c r="U26" s="196"/>
       <c r="AB26" s="47" t="str">
         <f>'2_PA'!U23</f>
         <v>Maggiolo Giorgio</v>
@@ -6430,7 +6431,7 @@
         <f>'2_PA'!AD23</f>
         <v>PA 3.3</v>
       </c>
-      <c r="AL26" s="184">
+      <c r="AL26" s="177">
         <f>'2_PA'!AE23</f>
         <v>28</v>
       </c>
@@ -6512,27 +6513,27 @@
       </c>
     </row>
     <row r="27" spans="1:60" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="183"/>
-      <c r="B27" s="181"/>
-      <c r="C27" s="181"/>
-      <c r="D27" s="181"/>
-      <c r="E27" s="181"/>
-      <c r="F27" s="181"/>
-      <c r="G27" s="181"/>
-      <c r="H27" s="181"/>
-      <c r="I27" s="181"/>
-      <c r="J27" s="181"/>
-      <c r="K27" s="182"/>
-      <c r="L27" s="182"/>
-      <c r="M27" s="182"/>
-      <c r="N27" s="181"/>
-      <c r="O27" s="181"/>
-      <c r="P27" s="181"/>
-      <c r="Q27" s="181"/>
-      <c r="R27" s="181"/>
-      <c r="S27" s="181"/>
-      <c r="T27" s="178"/>
-      <c r="U27" s="177"/>
+      <c r="A27" s="186"/>
+      <c r="B27" s="188"/>
+      <c r="C27" s="188"/>
+      <c r="D27" s="188"/>
+      <c r="E27" s="188"/>
+      <c r="F27" s="188"/>
+      <c r="G27" s="188"/>
+      <c r="H27" s="188"/>
+      <c r="I27" s="188"/>
+      <c r="J27" s="188"/>
+      <c r="K27" s="187"/>
+      <c r="L27" s="187"/>
+      <c r="M27" s="187"/>
+      <c r="N27" s="188"/>
+      <c r="O27" s="188"/>
+      <c r="P27" s="188"/>
+      <c r="Q27" s="188"/>
+      <c r="R27" s="188"/>
+      <c r="S27" s="188"/>
+      <c r="T27" s="197"/>
+      <c r="U27" s="196"/>
       <c r="AB27" s="63">
         <f>'2_PA'!U24</f>
         <v>0</v>
@@ -6573,7 +6574,7 @@
         <f>'2_PA'!AD24</f>
         <v>PA 5.1</v>
       </c>
-      <c r="AL27" s="198"/>
+      <c r="AL27" s="178"/>
       <c r="AO27">
         <f t="shared" si="35"/>
         <v>0</v>
@@ -6652,96 +6653,96 @@
       </c>
     </row>
     <row r="28" spans="1:60" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="183" t="s">
+      <c r="A28" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="181">
+      <c r="B28" s="188">
         <f>SUM(AO6:AQ6,AO18:AQ19,AO35:AQ36,AO52:AQ53)</f>
         <v>10</v>
       </c>
-      <c r="C28" s="181"/>
-      <c r="D28" s="181"/>
-      <c r="E28" s="181">
+      <c r="C28" s="188"/>
+      <c r="D28" s="188"/>
+      <c r="E28" s="188">
         <f>SUM(AR6:AT6,AR18:AT19,AR35:AT36,AR52:AT53)</f>
         <v>14</v>
       </c>
-      <c r="F28" s="181"/>
-      <c r="G28" s="181"/>
-      <c r="H28" s="181">
+      <c r="F28" s="188"/>
+      <c r="G28" s="188"/>
+      <c r="H28" s="188">
         <f>SUM(AU6:AW6,AU18:AW19,AU35:AW36,AU52:AW53)</f>
         <v>13</v>
       </c>
-      <c r="I28" s="181"/>
-      <c r="J28" s="181"/>
-      <c r="K28" s="181">
+      <c r="I28" s="188"/>
+      <c r="J28" s="188"/>
+      <c r="K28" s="188">
         <f>SUM(AX6:AZ6,AX18:AZ19,AX35:AZ36,AX52:AZ53)</f>
         <v>27</v>
       </c>
-      <c r="L28" s="181"/>
-      <c r="M28" s="181"/>
-      <c r="N28" s="181">
+      <c r="L28" s="188"/>
+      <c r="M28" s="188"/>
+      <c r="N28" s="188">
         <f>SUM(BA6:BC6,BA18:BC19,BA35:BC36,BA52:BC53)</f>
         <v>33</v>
       </c>
-      <c r="O28" s="181"/>
-      <c r="P28" s="181"/>
-      <c r="Q28" s="182">
+      <c r="O28" s="188"/>
+      <c r="P28" s="188"/>
+      <c r="Q28" s="187">
         <f>SUM(BD6:BF6,BD18:BF19,BD35:BF36,BD52:BF53)</f>
         <v>20</v>
       </c>
-      <c r="R28" s="182"/>
-      <c r="S28" s="182"/>
-      <c r="T28" s="178">
+      <c r="R28" s="187"/>
+      <c r="S28" s="187"/>
+      <c r="T28" s="197">
         <f t="shared" ref="T28" si="41">SUM(B28:S29)</f>
         <v>117</v>
       </c>
-      <c r="U28" s="177"/>
+      <c r="U28" s="196"/>
       <c r="BG28" s="158">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A29" s="183"/>
-      <c r="B29" s="181"/>
-      <c r="C29" s="181"/>
-      <c r="D29" s="181"/>
-      <c r="E29" s="181"/>
-      <c r="F29" s="181"/>
-      <c r="G29" s="181"/>
-      <c r="H29" s="181"/>
-      <c r="I29" s="181"/>
-      <c r="J29" s="181"/>
-      <c r="K29" s="181"/>
-      <c r="L29" s="181"/>
-      <c r="M29" s="181"/>
-      <c r="N29" s="181"/>
-      <c r="O29" s="181"/>
-      <c r="P29" s="181"/>
-      <c r="Q29" s="182"/>
-      <c r="R29" s="182"/>
-      <c r="S29" s="182"/>
-      <c r="T29" s="178"/>
-      <c r="U29" s="177"/>
+      <c r="A29" s="186"/>
+      <c r="B29" s="188"/>
+      <c r="C29" s="188"/>
+      <c r="D29" s="188"/>
+      <c r="E29" s="188"/>
+      <c r="F29" s="188"/>
+      <c r="G29" s="188"/>
+      <c r="H29" s="188"/>
+      <c r="I29" s="188"/>
+      <c r="J29" s="188"/>
+      <c r="K29" s="188"/>
+      <c r="L29" s="188"/>
+      <c r="M29" s="188"/>
+      <c r="N29" s="188"/>
+      <c r="O29" s="188"/>
+      <c r="P29" s="188"/>
+      <c r="Q29" s="187"/>
+      <c r="R29" s="187"/>
+      <c r="S29" s="187"/>
+      <c r="T29" s="197"/>
+      <c r="U29" s="196"/>
       <c r="AA29" t="s">
         <v>124</v>
       </c>
       <c r="AB29" s="149" t="s">
         <v>127</v>
       </c>
-      <c r="AC29" s="192" t="str">
+      <c r="AC29" s="179" t="str">
         <f>'3_PDC'!U6</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD29" s="193"/>
-      <c r="AE29" s="194"/>
-      <c r="AF29" s="192" t="str">
+      <c r="AD29" s="180"/>
+      <c r="AE29" s="181"/>
+      <c r="AF29" s="179" t="str">
         <f>'3_PDC'!X6</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG29" s="193"/>
-      <c r="AH29" s="195"/>
-      <c r="AI29" s="188" t="str">
+      <c r="AG29" s="180"/>
+      <c r="AH29" s="182"/>
+      <c r="AI29" s="183" t="str">
         <f>'3_PDC'!AA6</f>
         <v>Totale</v>
       </c>
@@ -6751,50 +6752,50 @@
       </c>
     </row>
     <row r="30" spans="1:60" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="183" t="s">
+      <c r="A30" s="186" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="181">
+      <c r="B30" s="188">
         <f>SUM(AO7:AQ7,AO20:AQ21,AO37:AQ38,AO54:AQ55)</f>
         <v>15</v>
       </c>
-      <c r="C30" s="181"/>
-      <c r="D30" s="181"/>
-      <c r="E30" s="181">
+      <c r="C30" s="188"/>
+      <c r="D30" s="188"/>
+      <c r="E30" s="188">
         <f>SUM(AR7:AT7,AR20:AT21,AR37:AT38,AR54:AT55)</f>
         <v>4</v>
       </c>
-      <c r="F30" s="181"/>
-      <c r="G30" s="181"/>
-      <c r="H30" s="181">
+      <c r="F30" s="188"/>
+      <c r="G30" s="188"/>
+      <c r="H30" s="188">
         <f>SUM(AU7:AW7,AU20:AW21,AU37:AW38,AU54:AW55)</f>
         <v>11</v>
       </c>
-      <c r="I30" s="181"/>
-      <c r="J30" s="181"/>
-      <c r="K30" s="182">
+      <c r="I30" s="188"/>
+      <c r="J30" s="188"/>
+      <c r="K30" s="187">
         <f>SUM(AX7:AZ7,AX20:AZ21,AX37:AZ38,AX54:AZ55)</f>
         <v>39</v>
       </c>
-      <c r="L30" s="182"/>
-      <c r="M30" s="182"/>
-      <c r="N30" s="182">
+      <c r="L30" s="187"/>
+      <c r="M30" s="187"/>
+      <c r="N30" s="187">
         <f>SUM(BA7:BC7,BA20:BC21,BA37:BC38,BA54:BC55)</f>
         <v>35</v>
       </c>
-      <c r="O30" s="182"/>
-      <c r="P30" s="182"/>
-      <c r="Q30" s="181">
+      <c r="O30" s="187"/>
+      <c r="P30" s="187"/>
+      <c r="Q30" s="188">
         <f>SUM(BD7:BF7,BD20:BF21,BD37:BF38,BD54:BF55)</f>
         <v>18</v>
       </c>
-      <c r="R30" s="181"/>
-      <c r="S30" s="181"/>
-      <c r="T30" s="178">
+      <c r="R30" s="188"/>
+      <c r="S30" s="188"/>
+      <c r="T30" s="197">
         <f t="shared" ref="T30" si="42">SUM(B30:S31)</f>
         <v>122</v>
       </c>
-      <c r="U30" s="177"/>
+      <c r="U30" s="196"/>
       <c r="AB30" s="150"/>
       <c r="AC30" s="26" t="str">
         <f>'3_PDC'!U7</f>
@@ -6820,7 +6821,7 @@
         <f>'3_PDC'!Z7</f>
         <v>Fase</v>
       </c>
-      <c r="AI30" s="189"/>
+      <c r="AI30" s="184"/>
       <c r="AK30">
         <f>SUM(AI31:AI44)</f>
         <v>373</v>
@@ -6831,27 +6832,27 @@
       </c>
     </row>
     <row r="31" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A31" s="183"/>
-      <c r="B31" s="181"/>
-      <c r="C31" s="181"/>
-      <c r="D31" s="181"/>
-      <c r="E31" s="181"/>
-      <c r="F31" s="181"/>
-      <c r="G31" s="181"/>
-      <c r="H31" s="181"/>
-      <c r="I31" s="181"/>
-      <c r="J31" s="181"/>
-      <c r="K31" s="182"/>
-      <c r="L31" s="182"/>
-      <c r="M31" s="182"/>
-      <c r="N31" s="182"/>
-      <c r="O31" s="182"/>
-      <c r="P31" s="182"/>
-      <c r="Q31" s="181"/>
-      <c r="R31" s="181"/>
-      <c r="S31" s="181"/>
-      <c r="T31" s="178"/>
-      <c r="U31" s="177"/>
+      <c r="A31" s="186"/>
+      <c r="B31" s="188"/>
+      <c r="C31" s="188"/>
+      <c r="D31" s="188"/>
+      <c r="E31" s="188"/>
+      <c r="F31" s="188"/>
+      <c r="G31" s="188"/>
+      <c r="H31" s="188"/>
+      <c r="I31" s="188"/>
+      <c r="J31" s="188"/>
+      <c r="K31" s="187"/>
+      <c r="L31" s="187"/>
+      <c r="M31" s="187"/>
+      <c r="N31" s="187"/>
+      <c r="O31" s="187"/>
+      <c r="P31" s="187"/>
+      <c r="Q31" s="188"/>
+      <c r="R31" s="188"/>
+      <c r="S31" s="188"/>
+      <c r="T31" s="197"/>
+      <c r="U31" s="196"/>
       <c r="AB31" s="31" t="str">
         <f>'3_PDC'!T8</f>
         <v>Begolo Marco</v>
@@ -6880,7 +6881,7 @@
         <f>'3_PDC'!Z8</f>
         <v>PDC 4.4</v>
       </c>
-      <c r="AI31" s="196">
+      <c r="AI31" s="185">
         <f>'3_PDC'!AA8</f>
         <v>52</v>
       </c>
@@ -6966,50 +6967,50 @@
       </c>
     </row>
     <row r="32" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A32" s="183" t="s">
+      <c r="A32" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="181">
+      <c r="B32" s="188">
         <f>SUM(AO8:AQ8,AO22:AQ23,AO39:AQ40,AO56:AQ57)</f>
         <v>9</v>
       </c>
-      <c r="C32" s="181"/>
-      <c r="D32" s="181"/>
-      <c r="E32" s="181">
+      <c r="C32" s="188"/>
+      <c r="D32" s="188"/>
+      <c r="E32" s="188">
         <f>SUM(AR8:AT8,AR22:AT23,AR39:AT40,AR56:AT57)</f>
         <v>11</v>
       </c>
-      <c r="F32" s="181"/>
-      <c r="G32" s="181"/>
-      <c r="H32" s="181">
+      <c r="F32" s="188"/>
+      <c r="G32" s="188"/>
+      <c r="H32" s="188">
         <f>SUM(AU8:AW8,AU22:AW23,AU39:AW40,AU56:AW57)</f>
         <v>12</v>
       </c>
-      <c r="I32" s="181"/>
-      <c r="J32" s="181"/>
-      <c r="K32" s="181">
+      <c r="I32" s="188"/>
+      <c r="J32" s="188"/>
+      <c r="K32" s="188">
         <f>SUM(AX8:AZ8,AX22:AZ23,AX39:AZ40,AX56:AZ57)</f>
         <v>30</v>
       </c>
-      <c r="L32" s="181"/>
-      <c r="M32" s="181"/>
-      <c r="N32" s="182">
+      <c r="L32" s="188"/>
+      <c r="M32" s="188"/>
+      <c r="N32" s="187">
         <f>SUM(BA8:BC8,BA22:BC23,BA39:BC40,BA56:BC57)</f>
         <v>37</v>
       </c>
-      <c r="O32" s="182"/>
-      <c r="P32" s="182"/>
-      <c r="Q32" s="181">
+      <c r="O32" s="187"/>
+      <c r="P32" s="187"/>
+      <c r="Q32" s="188">
         <f>SUM(BD8:BF8,BD22:BF23,BD39:BF40,BD56:BF57)</f>
         <v>23</v>
       </c>
-      <c r="R32" s="181"/>
-      <c r="S32" s="181"/>
-      <c r="T32" s="178">
+      <c r="R32" s="188"/>
+      <c r="S32" s="188"/>
+      <c r="T32" s="197">
         <f t="shared" ref="T32" si="58">SUM(B32:S33)</f>
         <v>122</v>
       </c>
-      <c r="U32" s="177"/>
+      <c r="U32" s="196"/>
       <c r="AB32" s="35">
         <f>'3_PDC'!T9</f>
         <v>0</v>
@@ -7038,7 +7039,7 @@
         <f>'3_PDC'!Z9</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI32" s="184"/>
+      <c r="AI32" s="177"/>
       <c r="AO32">
         <f>IF($AC32=AO$2,$AD32,0)</f>
         <v>0</v>
@@ -7117,27 +7118,27 @@
       </c>
     </row>
     <row r="33" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A33" s="183"/>
-      <c r="B33" s="181"/>
-      <c r="C33" s="181"/>
-      <c r="D33" s="181"/>
-      <c r="E33" s="181"/>
-      <c r="F33" s="181"/>
-      <c r="G33" s="181"/>
-      <c r="H33" s="181"/>
-      <c r="I33" s="181"/>
-      <c r="J33" s="181"/>
-      <c r="K33" s="181"/>
-      <c r="L33" s="181"/>
-      <c r="M33" s="181"/>
-      <c r="N33" s="182"/>
-      <c r="O33" s="182"/>
-      <c r="P33" s="182"/>
-      <c r="Q33" s="181"/>
-      <c r="R33" s="181"/>
-      <c r="S33" s="181"/>
-      <c r="T33" s="178"/>
-      <c r="U33" s="177"/>
+      <c r="A33" s="186"/>
+      <c r="B33" s="188"/>
+      <c r="C33" s="188"/>
+      <c r="D33" s="188"/>
+      <c r="E33" s="188"/>
+      <c r="F33" s="188"/>
+      <c r="G33" s="188"/>
+      <c r="H33" s="188"/>
+      <c r="I33" s="188"/>
+      <c r="J33" s="188"/>
+      <c r="K33" s="188"/>
+      <c r="L33" s="188"/>
+      <c r="M33" s="188"/>
+      <c r="N33" s="187"/>
+      <c r="O33" s="187"/>
+      <c r="P33" s="187"/>
+      <c r="Q33" s="188"/>
+      <c r="R33" s="188"/>
+      <c r="S33" s="188"/>
+      <c r="T33" s="197"/>
+      <c r="U33" s="196"/>
       <c r="AB33" s="31" t="str">
         <f>'3_PDC'!T10</f>
         <v>Facchin Gabriele</v>
@@ -7166,7 +7167,7 @@
         <f>'3_PDC'!Z10</f>
         <v>PDC 3.1</v>
       </c>
-      <c r="AI33" s="184">
+      <c r="AI33" s="177">
         <f>'3_PDC'!AA10</f>
         <v>52</v>
       </c>
@@ -7248,50 +7249,50 @@
       </c>
     </row>
     <row r="34" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A34" s="183" t="s">
+      <c r="A34" s="186" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="181">
+      <c r="B34" s="188">
         <f>SUM(AO9:AQ9,AO24:AQ25,AO41:AQ42,AO58:AQ59)</f>
         <v>6</v>
       </c>
-      <c r="C34" s="181"/>
-      <c r="D34" s="181"/>
-      <c r="E34" s="181">
+      <c r="C34" s="188"/>
+      <c r="D34" s="188"/>
+      <c r="E34" s="188">
         <f>SUM(AR9:AT9,AR24:AT25,AR41:AT42,AR58:AT59)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="181"/>
-      <c r="G34" s="181"/>
-      <c r="H34" s="181">
+      <c r="F34" s="188"/>
+      <c r="G34" s="188"/>
+      <c r="H34" s="188">
         <f>SUM(AU9:AW9,AU24:AW25,AU41:AW42,AU58:AW59)</f>
         <v>10</v>
       </c>
-      <c r="I34" s="181"/>
-      <c r="J34" s="181"/>
-      <c r="K34" s="182">
+      <c r="I34" s="188"/>
+      <c r="J34" s="188"/>
+      <c r="K34" s="187">
         <f>SUM(AX9:AZ9,AX24:AZ25,AX41:AZ42,AX58:AZ59)</f>
         <v>37</v>
       </c>
-      <c r="L34" s="182"/>
-      <c r="M34" s="182"/>
-      <c r="N34" s="182">
+      <c r="L34" s="187"/>
+      <c r="M34" s="187"/>
+      <c r="N34" s="187">
         <f>SUM(BA9:BC9,BA24:BC25,BA41:BC42,BA58:BC59)</f>
         <v>40</v>
       </c>
-      <c r="O34" s="182"/>
-      <c r="P34" s="182"/>
-      <c r="Q34" s="182">
+      <c r="O34" s="187"/>
+      <c r="P34" s="187"/>
+      <c r="Q34" s="187">
         <f>SUM(BD9:BF9,BD24:BF25,BD41:BF42,BD58:BF59)</f>
         <v>25</v>
       </c>
-      <c r="R34" s="182"/>
-      <c r="S34" s="182"/>
-      <c r="T34" s="178">
+      <c r="R34" s="187"/>
+      <c r="S34" s="187"/>
+      <c r="T34" s="197">
         <f t="shared" ref="T34" si="62">SUM(B34:S35)</f>
         <v>120</v>
       </c>
-      <c r="U34" s="177"/>
+      <c r="U34" s="196"/>
       <c r="AB34" s="31">
         <f>'3_PDC'!T11</f>
         <v>0</v>
@@ -7320,7 +7321,7 @@
         <f>'3_PDC'!Z11</f>
         <v>PDC 4.3</v>
       </c>
-      <c r="AI34" s="184"/>
+      <c r="AI34" s="177"/>
       <c r="AO34">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -7399,27 +7400,27 @@
       </c>
     </row>
     <row r="35" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A35" s="183"/>
-      <c r="B35" s="181"/>
-      <c r="C35" s="181"/>
-      <c r="D35" s="181"/>
-      <c r="E35" s="181"/>
-      <c r="F35" s="181"/>
-      <c r="G35" s="181"/>
-      <c r="H35" s="181"/>
-      <c r="I35" s="181"/>
-      <c r="J35" s="181"/>
-      <c r="K35" s="182"/>
-      <c r="L35" s="182"/>
-      <c r="M35" s="182"/>
-      <c r="N35" s="182"/>
-      <c r="O35" s="182"/>
-      <c r="P35" s="182"/>
-      <c r="Q35" s="182"/>
-      <c r="R35" s="182"/>
-      <c r="S35" s="182"/>
-      <c r="T35" s="178"/>
-      <c r="U35" s="177"/>
+      <c r="A35" s="186"/>
+      <c r="B35" s="188"/>
+      <c r="C35" s="188"/>
+      <c r="D35" s="188"/>
+      <c r="E35" s="188"/>
+      <c r="F35" s="188"/>
+      <c r="G35" s="188"/>
+      <c r="H35" s="188"/>
+      <c r="I35" s="188"/>
+      <c r="J35" s="188"/>
+      <c r="K35" s="187"/>
+      <c r="L35" s="187"/>
+      <c r="M35" s="187"/>
+      <c r="N35" s="187"/>
+      <c r="O35" s="187"/>
+      <c r="P35" s="187"/>
+      <c r="Q35" s="187"/>
+      <c r="R35" s="187"/>
+      <c r="S35" s="187"/>
+      <c r="T35" s="197"/>
+      <c r="U35" s="196"/>
       <c r="AB35" s="47" t="str">
         <f>'3_PDC'!T12</f>
         <v>Cornaglia Alessando</v>
@@ -7448,7 +7449,7 @@
         <f>'3_PDC'!Z12</f>
         <v>PDC 4.4 e 5</v>
       </c>
-      <c r="AI35" s="184">
+      <c r="AI35" s="177">
         <f>'3_PDC'!AA12</f>
         <v>52</v>
       </c>
@@ -7530,50 +7531,50 @@
       </c>
     </row>
     <row r="36" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A36" s="183" t="s">
+      <c r="A36" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="181">
+      <c r="B36" s="188">
         <f>SUM(AO10:AQ10,AO26:AQ27,AO43:AQ44,AO60:AQ61)</f>
         <v>12</v>
       </c>
-      <c r="C36" s="181"/>
-      <c r="D36" s="181"/>
-      <c r="E36" s="181">
+      <c r="C36" s="188"/>
+      <c r="D36" s="188"/>
+      <c r="E36" s="188">
         <f>SUM(AR10:AT10,AR26:AT27,AR43:AT44,AR60:AT61)</f>
         <v>18</v>
       </c>
-      <c r="F36" s="181"/>
-      <c r="G36" s="181"/>
-      <c r="H36" s="181">
+      <c r="F36" s="188"/>
+      <c r="G36" s="188"/>
+      <c r="H36" s="188">
         <f>SUM(AU10:AW10,AU26:AW27,AU43:AW44,AU60:AW61)</f>
         <v>7</v>
       </c>
-      <c r="I36" s="181"/>
-      <c r="J36" s="181"/>
-      <c r="K36" s="182">
+      <c r="I36" s="188"/>
+      <c r="J36" s="188"/>
+      <c r="K36" s="187">
         <f>SUM(AX10:AZ10,AX26:AZ27,AX43:AZ44,AX60:AZ61)</f>
         <v>51</v>
       </c>
-      <c r="L36" s="182"/>
-      <c r="M36" s="182"/>
-      <c r="N36" s="181">
+      <c r="L36" s="187"/>
+      <c r="M36" s="187"/>
+      <c r="N36" s="188">
         <f>SUM(BA10:BC10,BA26:BC27,BA43:BC44,BA60:BC61)</f>
         <v>10</v>
       </c>
-      <c r="O36" s="181"/>
-      <c r="P36" s="181"/>
-      <c r="Q36" s="181">
+      <c r="O36" s="188"/>
+      <c r="P36" s="188"/>
+      <c r="Q36" s="188">
         <f>SUM(BD10:BF10,BD26:BF27,BD43:BF44,BD60:BF61)</f>
         <v>18</v>
       </c>
-      <c r="R36" s="181"/>
-      <c r="S36" s="181"/>
-      <c r="T36" s="178">
+      <c r="R36" s="188"/>
+      <c r="S36" s="188"/>
+      <c r="T36" s="197">
         <f t="shared" ref="T36" si="63">SUM(B36:S37)</f>
         <v>116</v>
       </c>
-      <c r="U36" s="177"/>
+      <c r="U36" s="196"/>
       <c r="AB36" s="35">
         <f>'3_PDC'!T13</f>
         <v>0</v>
@@ -7602,7 +7603,7 @@
         <f>'3_PDC'!Z13</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI36" s="184"/>
+      <c r="AI36" s="177"/>
       <c r="AO36">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -7681,27 +7682,27 @@
       </c>
     </row>
     <row r="37" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A37" s="183"/>
-      <c r="B37" s="181"/>
-      <c r="C37" s="181"/>
-      <c r="D37" s="181"/>
-      <c r="E37" s="181"/>
-      <c r="F37" s="181"/>
-      <c r="G37" s="181"/>
-      <c r="H37" s="181"/>
-      <c r="I37" s="181"/>
-      <c r="J37" s="181"/>
-      <c r="K37" s="182"/>
-      <c r="L37" s="182"/>
-      <c r="M37" s="182"/>
-      <c r="N37" s="181"/>
-      <c r="O37" s="181"/>
-      <c r="P37" s="181"/>
-      <c r="Q37" s="181"/>
-      <c r="R37" s="181"/>
-      <c r="S37" s="181"/>
-      <c r="T37" s="178"/>
-      <c r="U37" s="177"/>
+      <c r="A37" s="186"/>
+      <c r="B37" s="188"/>
+      <c r="C37" s="188"/>
+      <c r="D37" s="188"/>
+      <c r="E37" s="188"/>
+      <c r="F37" s="188"/>
+      <c r="G37" s="188"/>
+      <c r="H37" s="188"/>
+      <c r="I37" s="188"/>
+      <c r="J37" s="188"/>
+      <c r="K37" s="187"/>
+      <c r="L37" s="187"/>
+      <c r="M37" s="187"/>
+      <c r="N37" s="188"/>
+      <c r="O37" s="188"/>
+      <c r="P37" s="188"/>
+      <c r="Q37" s="188"/>
+      <c r="R37" s="188"/>
+      <c r="S37" s="188"/>
+      <c r="T37" s="197"/>
+      <c r="U37" s="196"/>
       <c r="AB37" s="31" t="str">
         <f>'3_PDC'!T14</f>
         <v>Dalla Pietà Massimo</v>
@@ -7730,7 +7731,7 @@
         <f>'3_PDC'!Z14</f>
         <v>PDC 4.3</v>
       </c>
-      <c r="AI37" s="184">
+      <c r="AI37" s="177">
         <f>'3_PDC'!AA14</f>
         <v>57</v>
       </c>
@@ -7812,50 +7813,50 @@
       </c>
     </row>
     <row r="38" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A38" s="180" t="s">
+      <c r="A38" s="195" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="181">
+      <c r="B38" s="188">
         <f>SUM(B24:D37)</f>
         <v>82</v>
       </c>
-      <c r="C38" s="181"/>
-      <c r="D38" s="181"/>
-      <c r="E38" s="181">
+      <c r="C38" s="188"/>
+      <c r="D38" s="188"/>
+      <c r="E38" s="188">
         <f t="shared" ref="E38" si="64">SUM(E24:G37)</f>
         <v>69</v>
       </c>
-      <c r="F38" s="181"/>
-      <c r="G38" s="181"/>
-      <c r="H38" s="181">
+      <c r="F38" s="188"/>
+      <c r="G38" s="188"/>
+      <c r="H38" s="188">
         <f>SUM(H24:J37)</f>
         <v>79</v>
       </c>
-      <c r="I38" s="181"/>
-      <c r="J38" s="181"/>
-      <c r="K38" s="181">
+      <c r="I38" s="188"/>
+      <c r="J38" s="188"/>
+      <c r="K38" s="188">
         <f t="shared" ref="K38" si="65">SUM(K24:M37)</f>
         <v>235</v>
       </c>
-      <c r="L38" s="181"/>
-      <c r="M38" s="181"/>
-      <c r="N38" s="181">
+      <c r="L38" s="188"/>
+      <c r="M38" s="188"/>
+      <c r="N38" s="188">
         <f t="shared" ref="N38" si="66">SUM(N24:P37)</f>
         <v>243</v>
       </c>
-      <c r="O38" s="181"/>
-      <c r="P38" s="181"/>
-      <c r="Q38" s="181">
+      <c r="O38" s="188"/>
+      <c r="P38" s="188"/>
+      <c r="Q38" s="188">
         <f>SUM(Q24:S37)</f>
         <v>120</v>
       </c>
-      <c r="R38" s="181"/>
-      <c r="S38" s="181"/>
-      <c r="T38" s="179">
+      <c r="R38" s="188"/>
+      <c r="S38" s="188"/>
+      <c r="T38" s="198">
         <f>SUM(B38:S39)</f>
         <v>828</v>
       </c>
-      <c r="U38" s="177"/>
+      <c r="U38" s="196"/>
       <c r="AB38" s="31">
         <f>'3_PDC'!T15</f>
         <v>0</v>
@@ -7884,7 +7885,7 @@
         <f>'3_PDC'!Z15</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI38" s="184"/>
+      <c r="AI38" s="177"/>
       <c r="AO38">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -7963,27 +7964,27 @@
       </c>
     </row>
     <row r="39" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A39" s="180"/>
-      <c r="B39" s="181"/>
-      <c r="C39" s="181"/>
-      <c r="D39" s="181"/>
-      <c r="E39" s="181"/>
-      <c r="F39" s="181"/>
-      <c r="G39" s="181"/>
-      <c r="H39" s="181"/>
-      <c r="I39" s="181"/>
-      <c r="J39" s="181"/>
-      <c r="K39" s="181"/>
-      <c r="L39" s="181"/>
-      <c r="M39" s="181"/>
-      <c r="N39" s="181"/>
-      <c r="O39" s="181"/>
-      <c r="P39" s="181"/>
-      <c r="Q39" s="181"/>
-      <c r="R39" s="181"/>
-      <c r="S39" s="181"/>
-      <c r="T39" s="179"/>
-      <c r="U39" s="177"/>
+      <c r="A39" s="195"/>
+      <c r="B39" s="188"/>
+      <c r="C39" s="188"/>
+      <c r="D39" s="188"/>
+      <c r="E39" s="188"/>
+      <c r="F39" s="188"/>
+      <c r="G39" s="188"/>
+      <c r="H39" s="188"/>
+      <c r="I39" s="188"/>
+      <c r="J39" s="188"/>
+      <c r="K39" s="188"/>
+      <c r="L39" s="188"/>
+      <c r="M39" s="188"/>
+      <c r="N39" s="188"/>
+      <c r="O39" s="188"/>
+      <c r="P39" s="188"/>
+      <c r="Q39" s="188"/>
+      <c r="R39" s="188"/>
+      <c r="S39" s="188"/>
+      <c r="T39" s="198"/>
+      <c r="U39" s="196"/>
       <c r="AB39" s="47" t="str">
         <f>'3_PDC'!T16</f>
         <v>Braghetto Lorenzo</v>
@@ -8012,7 +8013,7 @@
         <f>'3_PDC'!Z16</f>
         <v>PDC 4.4</v>
       </c>
-      <c r="AI39" s="184">
+      <c r="AI39" s="177">
         <f>'3_PDC'!AA16</f>
         <v>54</v>
       </c>
@@ -8123,7 +8124,7 @@
         <f>'3_PDC'!Z17</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI40" s="184"/>
+      <c r="AI40" s="177"/>
       <c r="AO40">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -8231,7 +8232,7 @@
         <f>'3_PDC'!Z18</f>
         <v>PDC 6</v>
       </c>
-      <c r="AI41" s="184">
+      <c r="AI41" s="177">
         <f>'3_PDC'!AA18</f>
         <v>54</v>
       </c>
@@ -8342,7 +8343,7 @@
         <f>'3_PDC'!Z19</f>
         <v>PDC 3.2, 5 e 7</v>
       </c>
-      <c r="AI42" s="184"/>
+      <c r="AI42" s="177"/>
       <c r="AO42">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -8450,7 +8451,7 @@
         <f>'3_PDC'!Z20</f>
         <v>PDC 4.3</v>
       </c>
-      <c r="AI43" s="184">
+      <c r="AI43" s="177">
         <f>'3_PDC'!AA20</f>
         <v>52</v>
       </c>
@@ -8561,7 +8562,7 @@
         <f>'3_PDC'!Z21</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI44" s="198"/>
+      <c r="AI44" s="178"/>
       <c r="AO44">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -8654,19 +8655,19 @@
       <c r="AB46" s="149" t="s">
         <v>128</v>
       </c>
-      <c r="AC46" s="192" t="str">
+      <c r="AC46" s="179" t="str">
         <f>'4_VV'!U3</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD46" s="193"/>
-      <c r="AE46" s="194"/>
-      <c r="AF46" s="192" t="str">
+      <c r="AD46" s="180"/>
+      <c r="AE46" s="181"/>
+      <c r="AF46" s="179" t="str">
         <f>'4_VV'!X3</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG46" s="193"/>
-      <c r="AH46" s="195"/>
-      <c r="AI46" s="188" t="str">
+      <c r="AG46" s="180"/>
+      <c r="AH46" s="182"/>
+      <c r="AI46" s="183" t="str">
         <f>'4_VV'!AA3</f>
         <v>Totale</v>
       </c>
@@ -8706,7 +8707,7 @@
         <f>'4_VV'!Z4</f>
         <v>Fase</v>
       </c>
-      <c r="AI47" s="189"/>
+      <c r="AI47" s="184"/>
       <c r="BG47" s="158">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -8742,7 +8743,7 @@
         <f>'4_VV'!Z5</f>
         <v>VV 3.2</v>
       </c>
-      <c r="AI48" s="196">
+      <c r="AI48" s="185">
         <f>'4_VV'!AA5</f>
         <v>18</v>
       </c>
@@ -8856,7 +8857,7 @@
         <f>'4_VV'!Z6</f>
         <v>0</v>
       </c>
-      <c r="AI49" s="184"/>
+      <c r="AI49" s="177"/>
       <c r="AO49">
         <f>IF($AC49=AO$2,$AD49,0)</f>
         <v>0</v>
@@ -8963,7 +8964,7 @@
         <f>'4_VV'!Z7</f>
         <v>VV 3.2</v>
       </c>
-      <c r="AI50" s="184">
+      <c r="AI50" s="177">
         <f>'4_VV'!AA7</f>
         <v>18</v>
       </c>
@@ -9085,7 +9086,7 @@
         <f>'4_VV'!Z8</f>
         <v>VV 3.2</v>
       </c>
-      <c r="AI51" s="184"/>
+      <c r="AI51" s="177"/>
       <c r="AO51">
         <f t="shared" si="82"/>
         <v>0</v>
@@ -9206,7 +9207,7 @@
         <f>'4_VV'!Z9</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI52" s="184">
+      <c r="AI52" s="177">
         <f>'4_VV'!AA9</f>
         <v>18</v>
       </c>
@@ -9330,7 +9331,7 @@
         <f>'4_VV'!Z10</f>
         <v>0</v>
       </c>
-      <c r="AI53" s="184"/>
+      <c r="AI53" s="177"/>
       <c r="AO53">
         <f t="shared" si="82"/>
         <v>0</v>
@@ -9451,7 +9452,7 @@
         <f>'4_VV'!Z11</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI54" s="184">
+      <c r="AI54" s="177">
         <f>'4_VV'!AA11</f>
         <v>18</v>
       </c>
@@ -9575,7 +9576,7 @@
         <f>'4_VV'!Z12</f>
         <v>0</v>
       </c>
-      <c r="AI55" s="184"/>
+      <c r="AI55" s="177"/>
       <c r="AO55">
         <f t="shared" si="82"/>
         <v>0</v>
@@ -9696,7 +9697,7 @@
         <f>'4_VV'!Z13</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI56" s="184">
+      <c r="AI56" s="177">
         <f>'4_VV'!AA13</f>
         <v>18</v>
       </c>
@@ -9820,7 +9821,7 @@
         <f>'4_VV'!Z14</f>
         <v>0</v>
       </c>
-      <c r="AI57" s="184"/>
+      <c r="AI57" s="177"/>
       <c r="AO57">
         <f t="shared" si="82"/>
         <v>0</v>
@@ -9938,7 +9939,7 @@
         <f>'4_VV'!Z15</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI58" s="184">
+      <c r="AI58" s="177">
         <f>'4_VV'!AA15</f>
         <v>18</v>
       </c>
@@ -10048,7 +10049,7 @@
         <f>'4_VV'!Z16</f>
         <v>0</v>
       </c>
-      <c r="AI59" s="184"/>
+      <c r="AI59" s="177"/>
       <c r="AO59">
         <f t="shared" si="82"/>
         <v>0</v>
@@ -10155,7 +10156,7 @@
         <f>'4_VV'!Z17</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI60" s="184">
+      <c r="AI60" s="177">
         <f>'4_VV'!AA17</f>
         <v>16</v>
       </c>
@@ -10265,7 +10266,7 @@
         <f>'4_VV'!Z18</f>
         <v>0</v>
       </c>
-      <c r="AI61" s="198"/>
+      <c r="AI61" s="178"/>
       <c r="AO61">
         <f t="shared" si="82"/>
         <v>0</v>
@@ -10345,78 +10346,22 @@
     </row>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="AI43:AI44"/>
-    <mergeCell ref="AC46:AE46"/>
-    <mergeCell ref="AF46:AH46"/>
-    <mergeCell ref="AI46:AI47"/>
-    <mergeCell ref="AI60:AI61"/>
-    <mergeCell ref="AI48:AI49"/>
-    <mergeCell ref="AI50:AI51"/>
-    <mergeCell ref="AI52:AI53"/>
-    <mergeCell ref="AI54:AI55"/>
-    <mergeCell ref="AI56:AI57"/>
-    <mergeCell ref="AI58:AI59"/>
-    <mergeCell ref="AI41:AI42"/>
-    <mergeCell ref="AL24:AL25"/>
-    <mergeCell ref="AL26:AL27"/>
-    <mergeCell ref="AC29:AE29"/>
-    <mergeCell ref="AF29:AH29"/>
-    <mergeCell ref="AI29:AI30"/>
-    <mergeCell ref="AI31:AI32"/>
-    <mergeCell ref="AI33:AI34"/>
-    <mergeCell ref="AI35:AI36"/>
-    <mergeCell ref="AI37:AI38"/>
-    <mergeCell ref="AI39:AI40"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="H24:J25"/>
-    <mergeCell ref="E24:G25"/>
-    <mergeCell ref="B24:D25"/>
-    <mergeCell ref="AL22:AL23"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AC12:AE12"/>
-    <mergeCell ref="AF12:AH12"/>
-    <mergeCell ref="AI12:AK12"/>
-    <mergeCell ref="AL12:AL13"/>
-    <mergeCell ref="AL14:AL15"/>
-    <mergeCell ref="AL16:AL17"/>
-    <mergeCell ref="AL18:AL19"/>
-    <mergeCell ref="AL20:AL21"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:D27"/>
-    <mergeCell ref="E26:G27"/>
-    <mergeCell ref="H26:J27"/>
-    <mergeCell ref="K26:M27"/>
-    <mergeCell ref="E30:G31"/>
-    <mergeCell ref="H30:J31"/>
-    <mergeCell ref="K30:M31"/>
-    <mergeCell ref="N26:P27"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="K32:M33"/>
-    <mergeCell ref="N32:P33"/>
-    <mergeCell ref="Q32:S33"/>
-    <mergeCell ref="Q24:S25"/>
-    <mergeCell ref="N24:P25"/>
-    <mergeCell ref="K24:M25"/>
-    <mergeCell ref="B32:D33"/>
-    <mergeCell ref="E32:G33"/>
-    <mergeCell ref="H32:J33"/>
-    <mergeCell ref="Q26:S27"/>
-    <mergeCell ref="K28:M29"/>
-    <mergeCell ref="N28:P29"/>
-    <mergeCell ref="Q28:S29"/>
-    <mergeCell ref="B30:D31"/>
-    <mergeCell ref="B28:D29"/>
-    <mergeCell ref="E28:G29"/>
-    <mergeCell ref="H28:J29"/>
+    <mergeCell ref="U38:U39"/>
+    <mergeCell ref="U34:U35"/>
+    <mergeCell ref="U32:U33"/>
+    <mergeCell ref="U30:U31"/>
+    <mergeCell ref="U28:U29"/>
+    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="U36:U37"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="T24:T25"/>
+    <mergeCell ref="T34:T35"/>
+    <mergeCell ref="T32:T33"/>
+    <mergeCell ref="T30:T31"/>
+    <mergeCell ref="T28:T29"/>
+    <mergeCell ref="T38:T39"/>
+    <mergeCell ref="T36:T37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:D39"/>
     <mergeCell ref="E38:G39"/>
@@ -10441,22 +10386,78 @@
     <mergeCell ref="N36:P37"/>
     <mergeCell ref="Q36:S37"/>
     <mergeCell ref="Q34:S35"/>
-    <mergeCell ref="U38:U39"/>
-    <mergeCell ref="U34:U35"/>
-    <mergeCell ref="U32:U33"/>
-    <mergeCell ref="U30:U31"/>
-    <mergeCell ref="U28:U29"/>
-    <mergeCell ref="U26:U27"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="U36:U37"/>
-    <mergeCell ref="T26:T27"/>
-    <mergeCell ref="T24:T25"/>
-    <mergeCell ref="T34:T35"/>
-    <mergeCell ref="T32:T33"/>
-    <mergeCell ref="T30:T31"/>
-    <mergeCell ref="T28:T29"/>
-    <mergeCell ref="T38:T39"/>
-    <mergeCell ref="T36:T37"/>
+    <mergeCell ref="K32:M33"/>
+    <mergeCell ref="N32:P33"/>
+    <mergeCell ref="Q32:S33"/>
+    <mergeCell ref="Q24:S25"/>
+    <mergeCell ref="N24:P25"/>
+    <mergeCell ref="K24:M25"/>
+    <mergeCell ref="B32:D33"/>
+    <mergeCell ref="E32:G33"/>
+    <mergeCell ref="H32:J33"/>
+    <mergeCell ref="Q26:S27"/>
+    <mergeCell ref="K28:M29"/>
+    <mergeCell ref="N28:P29"/>
+    <mergeCell ref="Q28:S29"/>
+    <mergeCell ref="B30:D31"/>
+    <mergeCell ref="B28:D29"/>
+    <mergeCell ref="E28:G29"/>
+    <mergeCell ref="H28:J29"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:D27"/>
+    <mergeCell ref="E26:G27"/>
+    <mergeCell ref="H26:J27"/>
+    <mergeCell ref="K26:M27"/>
+    <mergeCell ref="E30:G31"/>
+    <mergeCell ref="H30:J31"/>
+    <mergeCell ref="K30:M31"/>
+    <mergeCell ref="N26:P27"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="H24:J25"/>
+    <mergeCell ref="E24:G25"/>
+    <mergeCell ref="B24:D25"/>
+    <mergeCell ref="AL22:AL23"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AC12:AE12"/>
+    <mergeCell ref="AF12:AH12"/>
+    <mergeCell ref="AI12:AK12"/>
+    <mergeCell ref="AL12:AL13"/>
+    <mergeCell ref="AL14:AL15"/>
+    <mergeCell ref="AL16:AL17"/>
+    <mergeCell ref="AL18:AL19"/>
+    <mergeCell ref="AL20:AL21"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="AI41:AI42"/>
+    <mergeCell ref="AL24:AL25"/>
+    <mergeCell ref="AL26:AL27"/>
+    <mergeCell ref="AC29:AE29"/>
+    <mergeCell ref="AF29:AH29"/>
+    <mergeCell ref="AI29:AI30"/>
+    <mergeCell ref="AI31:AI32"/>
+    <mergeCell ref="AI33:AI34"/>
+    <mergeCell ref="AI35:AI36"/>
+    <mergeCell ref="AI37:AI38"/>
+    <mergeCell ref="AI39:AI40"/>
+    <mergeCell ref="AI43:AI44"/>
+    <mergeCell ref="AC46:AE46"/>
+    <mergeCell ref="AF46:AH46"/>
+    <mergeCell ref="AI46:AI47"/>
+    <mergeCell ref="AI60:AI61"/>
+    <mergeCell ref="AI48:AI49"/>
+    <mergeCell ref="AI50:AI51"/>
+    <mergeCell ref="AI52:AI53"/>
+    <mergeCell ref="AI54:AI55"/>
+    <mergeCell ref="AI56:AI57"/>
+    <mergeCell ref="AI58:AI59"/>
   </mergeCells>
   <conditionalFormatting sqref="AB14:AL27">
     <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
@@ -10567,13 +10568,13 @@
         <v>74</v>
       </c>
       <c r="AB2" s="149"/>
-      <c r="AC2" s="185"/>
-      <c r="AD2" s="186"/>
-      <c r="AE2" s="187"/>
-      <c r="AF2" s="185"/>
-      <c r="AG2" s="186"/>
-      <c r="AH2" s="186"/>
-      <c r="AI2" s="188"/>
+      <c r="AC2" s="189"/>
+      <c r="AD2" s="190"/>
+      <c r="AE2" s="191"/>
+      <c r="AF2" s="189"/>
+      <c r="AG2" s="190"/>
+      <c r="AH2" s="190"/>
+      <c r="AI2" s="183"/>
       <c r="AJ2">
         <f>SUM(AI4:AI10)</f>
         <v>0</v>
@@ -10663,7 +10664,7 @@
       <c r="AF3" s="104"/>
       <c r="AG3" s="105"/>
       <c r="AH3" s="107"/>
-      <c r="AI3" s="189"/>
+      <c r="AI3" s="184"/>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="147"/>
@@ -11276,25 +11277,25 @@
       <c r="AB12" s="149" t="s">
         <v>126</v>
       </c>
-      <c r="AC12" s="185" t="str">
+      <c r="AC12" s="189" t="str">
         <f>'2_PA'!V9</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD12" s="190"/>
-      <c r="AE12" s="191"/>
-      <c r="AF12" s="192" t="str">
+      <c r="AD12" s="192"/>
+      <c r="AE12" s="193"/>
+      <c r="AF12" s="179" t="str">
         <f>'2_PA'!Y9</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG12" s="193"/>
-      <c r="AH12" s="194"/>
-      <c r="AI12" s="192" t="str">
+      <c r="AG12" s="180"/>
+      <c r="AH12" s="181"/>
+      <c r="AI12" s="179" t="str">
         <f>'2_PA'!AB9</f>
         <v>III Periodo</v>
       </c>
-      <c r="AJ12" s="193"/>
-      <c r="AK12" s="195"/>
-      <c r="AL12" s="188" t="str">
+      <c r="AJ12" s="180"/>
+      <c r="AK12" s="182"/>
+      <c r="AL12" s="183" t="str">
         <f>'2_PA'!AE9</f>
         <v>Totale</v>
       </c>
@@ -11341,7 +11342,7 @@
         <f>'2_PA'!AD10</f>
         <v>Fase</v>
       </c>
-      <c r="AL13" s="189"/>
+      <c r="AL13" s="184"/>
       <c r="AM13">
         <f>SUM(AL14:AL27)</f>
         <v>193</v>
@@ -11392,7 +11393,7 @@
         <f>'2_PA'!AD11</f>
         <v>PA 3.2</v>
       </c>
-      <c r="AL14" s="196">
+      <c r="AL14" s="185">
         <f>'2_PA'!AE11</f>
         <v>26</v>
       </c>
@@ -11518,7 +11519,7 @@
         <f>'2_PA'!AD12</f>
         <v>0</v>
       </c>
-      <c r="AL15" s="184"/>
+      <c r="AL15" s="177"/>
       <c r="AO15">
         <f>IF($AC15=AO$2,$AD15,0)</f>
         <v>0</v>
@@ -11637,7 +11638,7 @@
         <f>'2_PA'!AD13</f>
         <v>PA 3.2</v>
       </c>
-      <c r="AL16" s="184">
+      <c r="AL16" s="177">
         <f>'2_PA'!AE13</f>
         <v>27</v>
       </c>
@@ -11759,7 +11760,7 @@
         <f>'2_PA'!AD14</f>
         <v>0</v>
       </c>
-      <c r="AL17" s="184"/>
+      <c r="AL17" s="177"/>
       <c r="AO17">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -11878,7 +11879,7 @@
         <f>'2_PA'!AD15</f>
         <v>PA 3.3</v>
       </c>
-      <c r="AL18" s="184">
+      <c r="AL18" s="177">
         <f>'2_PA'!AE15</f>
         <v>26</v>
       </c>
@@ -12000,7 +12001,7 @@
         <f>'2_PA'!AD16</f>
         <v>PA 6.1</v>
       </c>
-      <c r="AL19" s="184"/>
+      <c r="AL19" s="177"/>
       <c r="AO19">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -12119,7 +12120,7 @@
         <f>'2_PA'!AD17</f>
         <v>PA 3.3</v>
       </c>
-      <c r="AL20" s="184">
+      <c r="AL20" s="177">
         <f>'2_PA'!AE17</f>
         <v>28</v>
       </c>
@@ -12241,7 +12242,7 @@
         <f>'2_PA'!AD18</f>
         <v>PA 6.2</v>
       </c>
-      <c r="AL21" s="184"/>
+      <c r="AL21" s="177"/>
       <c r="AO21">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -12360,7 +12361,7 @@
         <f>'2_PA'!AD19</f>
         <v>PA 5.1</v>
       </c>
-      <c r="AL22" s="184">
+      <c r="AL22" s="177">
         <f>'2_PA'!AE19</f>
         <v>30</v>
       </c>
@@ -12445,36 +12446,36 @@
       <c r="A23" s="156" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="197" t="s">
+      <c r="B23" s="194" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="197"/>
-      <c r="D23" s="197"/>
-      <c r="E23" s="197" t="s">
+      <c r="C23" s="194"/>
+      <c r="D23" s="194"/>
+      <c r="E23" s="194" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="197"/>
-      <c r="G23" s="197"/>
-      <c r="H23" s="197" t="s">
+      <c r="F23" s="194"/>
+      <c r="G23" s="194"/>
+      <c r="H23" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="I23" s="197"/>
-      <c r="J23" s="197"/>
-      <c r="K23" s="197" t="s">
+      <c r="I23" s="194"/>
+      <c r="J23" s="194"/>
+      <c r="K23" s="194" t="s">
         <v>4</v>
       </c>
-      <c r="L23" s="197"/>
-      <c r="M23" s="197"/>
-      <c r="N23" s="197" t="s">
+      <c r="L23" s="194"/>
+      <c r="M23" s="194"/>
+      <c r="N23" s="194" t="s">
         <v>5</v>
       </c>
-      <c r="O23" s="197"/>
-      <c r="P23" s="197"/>
-      <c r="Q23" s="197" t="s">
+      <c r="O23" s="194"/>
+      <c r="P23" s="194"/>
+      <c r="Q23" s="194" t="s">
         <v>6</v>
       </c>
-      <c r="R23" s="197"/>
-      <c r="S23" s="197"/>
+      <c r="R23" s="194"/>
+      <c r="S23" s="194"/>
       <c r="T23" s="156" t="s">
         <v>14</v>
       </c>
@@ -12519,7 +12520,7 @@
         <f>'2_PA'!AD20</f>
         <v>0</v>
       </c>
-      <c r="AL23" s="184"/>
+      <c r="AL23" s="177"/>
       <c r="AO23">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -12598,50 +12599,50 @@
       </c>
     </row>
     <row r="24" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A24" s="183" t="s">
+      <c r="A24" s="186" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="181">
+      <c r="B24" s="188">
         <f>SUM(AO4:AQ4,AO14:AQ15,AO31:AQ32,AO48:AQ49)</f>
         <v>4</v>
       </c>
-      <c r="C24" s="181"/>
-      <c r="D24" s="181"/>
-      <c r="E24" s="181">
+      <c r="C24" s="188"/>
+      <c r="D24" s="188"/>
+      <c r="E24" s="188">
         <f>SUM(AR4:AT4,AR14:AT15,AR31:AT32,AR48:AT49)</f>
         <v>10</v>
       </c>
-      <c r="F24" s="181"/>
-      <c r="G24" s="181"/>
-      <c r="H24" s="182">
+      <c r="F24" s="188"/>
+      <c r="G24" s="188"/>
+      <c r="H24" s="187">
         <f>SUM(AU4:AW4,AU14:AW15,AU31:AW32,AU48:AW49)</f>
         <v>9</v>
       </c>
-      <c r="I24" s="182"/>
-      <c r="J24" s="182"/>
-      <c r="K24" s="181">
+      <c r="I24" s="187"/>
+      <c r="J24" s="187"/>
+      <c r="K24" s="188">
         <f>SUM(AX4:AZ4,AX14:AZ15,AX31:AZ32,AX48:AZ49)</f>
         <v>10</v>
       </c>
-      <c r="L24" s="181"/>
-      <c r="M24" s="181"/>
-      <c r="N24" s="182">
+      <c r="L24" s="188"/>
+      <c r="M24" s="188"/>
+      <c r="N24" s="187">
         <f>SUM(BA4:BC4,BA14:BC15,BA31:BC32,BA48:BC49)</f>
         <v>59</v>
       </c>
-      <c r="O24" s="182"/>
-      <c r="P24" s="182"/>
-      <c r="Q24" s="181">
+      <c r="O24" s="187"/>
+      <c r="P24" s="187"/>
+      <c r="Q24" s="188">
         <f>SUM(BD4:BF4,BD14:BF15,BD31:BF32,BD48:BF49)</f>
         <v>4</v>
       </c>
-      <c r="R24" s="181"/>
-      <c r="S24" s="181"/>
-      <c r="T24" s="181">
+      <c r="R24" s="188"/>
+      <c r="S24" s="188"/>
+      <c r="T24" s="188">
         <f t="shared" ref="T24" si="32">SUM(B24:S25)</f>
         <v>96</v>
       </c>
-      <c r="U24" s="177"/>
+      <c r="U24" s="196"/>
       <c r="AB24" s="31" t="str">
         <f>'2_PA'!U21</f>
         <v>Quadrio Giacomo</v>
@@ -12682,7 +12683,7 @@
         <f>'2_PA'!AD21</f>
         <v>PA 5.1, 6.2</v>
       </c>
-      <c r="AL24" s="184">
+      <c r="AL24" s="177">
         <f>'2_PA'!AE21</f>
         <v>28</v>
       </c>
@@ -12764,27 +12765,27 @@
       </c>
     </row>
     <row r="25" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A25" s="183"/>
-      <c r="B25" s="181"/>
-      <c r="C25" s="181"/>
-      <c r="D25" s="181"/>
-      <c r="E25" s="181"/>
-      <c r="F25" s="181"/>
-      <c r="G25" s="181"/>
-      <c r="H25" s="182"/>
-      <c r="I25" s="182"/>
-      <c r="J25" s="182"/>
-      <c r="K25" s="181"/>
-      <c r="L25" s="181"/>
-      <c r="M25" s="181"/>
-      <c r="N25" s="182"/>
-      <c r="O25" s="182"/>
-      <c r="P25" s="182"/>
-      <c r="Q25" s="181"/>
-      <c r="R25" s="181"/>
-      <c r="S25" s="181"/>
-      <c r="T25" s="181"/>
-      <c r="U25" s="177"/>
+      <c r="A25" s="186"/>
+      <c r="B25" s="188"/>
+      <c r="C25" s="188"/>
+      <c r="D25" s="188"/>
+      <c r="E25" s="188"/>
+      <c r="F25" s="188"/>
+      <c r="G25" s="188"/>
+      <c r="H25" s="187"/>
+      <c r="I25" s="187"/>
+      <c r="J25" s="187"/>
+      <c r="K25" s="188"/>
+      <c r="L25" s="188"/>
+      <c r="M25" s="188"/>
+      <c r="N25" s="187"/>
+      <c r="O25" s="187"/>
+      <c r="P25" s="187"/>
+      <c r="Q25" s="188"/>
+      <c r="R25" s="188"/>
+      <c r="S25" s="188"/>
+      <c r="T25" s="188"/>
+      <c r="U25" s="196"/>
       <c r="AB25" s="31">
         <f>'2_PA'!U22</f>
         <v>0</v>
@@ -12825,7 +12826,7 @@
         <f>'2_PA'!AD22</f>
         <v>0</v>
       </c>
-      <c r="AL25" s="184"/>
+      <c r="AL25" s="177"/>
       <c r="AO25">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -12904,50 +12905,50 @@
       </c>
     </row>
     <row r="26" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A26" s="183" t="s">
+      <c r="A26" s="186" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="181">
+      <c r="B26" s="188">
         <f>SUM(AO5:AQ5,AO16:AQ17,AO33:AQ34,AO50:AQ51)</f>
         <v>13</v>
       </c>
-      <c r="C26" s="181"/>
-      <c r="D26" s="181"/>
-      <c r="E26" s="181">
+      <c r="C26" s="188"/>
+      <c r="D26" s="188"/>
+      <c r="E26" s="188">
         <f>SUM(AR5:AT5,AR16:AT17,AR33:AT34,AR50:AT51)</f>
         <v>10</v>
       </c>
-      <c r="F26" s="181"/>
-      <c r="G26" s="181"/>
-      <c r="H26" s="181">
+      <c r="F26" s="188"/>
+      <c r="G26" s="188"/>
+      <c r="H26" s="188">
         <f>SUM(AU5:AW5,AU16:AW17,AU33:AW34,AU50:AW51)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="181"/>
-      <c r="J26" s="181"/>
-      <c r="K26" s="182">
+      <c r="I26" s="188"/>
+      <c r="J26" s="188"/>
+      <c r="K26" s="187">
         <f>SUM(AX5:AZ5,AX16:AZ17,AX33:AZ34,AX50:AZ51)</f>
         <v>33</v>
       </c>
-      <c r="L26" s="182"/>
-      <c r="M26" s="182"/>
-      <c r="N26" s="181">
+      <c r="L26" s="187"/>
+      <c r="M26" s="187"/>
+      <c r="N26" s="188">
         <f>SUM(BA5:BC5,BA16:BC17,BA33:BC34,BA50:BC51)</f>
         <v>29</v>
       </c>
-      <c r="O26" s="181"/>
-      <c r="P26" s="181"/>
-      <c r="Q26" s="181">
+      <c r="O26" s="188"/>
+      <c r="P26" s="188"/>
+      <c r="Q26" s="188">
         <f>SUM(BD5:BF5,BD16:BF17,BD33:BF34,BD50:BF51)</f>
         <v>12</v>
       </c>
-      <c r="R26" s="181"/>
-      <c r="S26" s="181"/>
-      <c r="T26" s="181">
+      <c r="R26" s="188"/>
+      <c r="S26" s="188"/>
+      <c r="T26" s="188">
         <f t="shared" ref="T26" si="33">SUM(B26:S27)</f>
         <v>97</v>
       </c>
-      <c r="U26" s="177"/>
+      <c r="U26" s="196"/>
       <c r="AB26" s="47" t="str">
         <f>'2_PA'!U23</f>
         <v>Maggiolo Giorgio</v>
@@ -12988,7 +12989,7 @@
         <f>'2_PA'!AD23</f>
         <v>PA 3.3</v>
       </c>
-      <c r="AL26" s="184">
+      <c r="AL26" s="177">
         <f>'2_PA'!AE23</f>
         <v>28</v>
       </c>
@@ -13070,27 +13071,27 @@
       </c>
     </row>
     <row r="27" spans="1:60" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="183"/>
-      <c r="B27" s="181"/>
-      <c r="C27" s="181"/>
-      <c r="D27" s="181"/>
-      <c r="E27" s="181"/>
-      <c r="F27" s="181"/>
-      <c r="G27" s="181"/>
-      <c r="H27" s="181"/>
-      <c r="I27" s="181"/>
-      <c r="J27" s="181"/>
-      <c r="K27" s="182"/>
-      <c r="L27" s="182"/>
-      <c r="M27" s="182"/>
-      <c r="N27" s="181"/>
-      <c r="O27" s="181"/>
-      <c r="P27" s="181"/>
-      <c r="Q27" s="181"/>
-      <c r="R27" s="181"/>
-      <c r="S27" s="181"/>
-      <c r="T27" s="181"/>
-      <c r="U27" s="177"/>
+      <c r="A27" s="186"/>
+      <c r="B27" s="188"/>
+      <c r="C27" s="188"/>
+      <c r="D27" s="188"/>
+      <c r="E27" s="188"/>
+      <c r="F27" s="188"/>
+      <c r="G27" s="188"/>
+      <c r="H27" s="188"/>
+      <c r="I27" s="188"/>
+      <c r="J27" s="188"/>
+      <c r="K27" s="187"/>
+      <c r="L27" s="187"/>
+      <c r="M27" s="187"/>
+      <c r="N27" s="188"/>
+      <c r="O27" s="188"/>
+      <c r="P27" s="188"/>
+      <c r="Q27" s="188"/>
+      <c r="R27" s="188"/>
+      <c r="S27" s="188"/>
+      <c r="T27" s="188"/>
+      <c r="U27" s="196"/>
       <c r="AB27" s="63">
         <f>'2_PA'!U24</f>
         <v>0</v>
@@ -13131,7 +13132,7 @@
         <f>'2_PA'!AD24</f>
         <v>PA 5.1</v>
       </c>
-      <c r="AL27" s="198"/>
+      <c r="AL27" s="178"/>
       <c r="AO27">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -13210,96 +13211,96 @@
       </c>
     </row>
     <row r="28" spans="1:60" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="183" t="s">
+      <c r="A28" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="181">
+      <c r="B28" s="188">
         <f>SUM(AO6:AQ6,AO18:AQ19,AO35:AQ36,AO52:AQ53)</f>
         <v>10</v>
       </c>
-      <c r="C28" s="181"/>
-      <c r="D28" s="181"/>
-      <c r="E28" s="181">
+      <c r="C28" s="188"/>
+      <c r="D28" s="188"/>
+      <c r="E28" s="188">
         <f>SUM(AR6:AT6,AR18:AT19,AR35:AT36,AR52:AT53)</f>
         <v>4</v>
       </c>
-      <c r="F28" s="181"/>
-      <c r="G28" s="181"/>
-      <c r="H28" s="181">
+      <c r="F28" s="188"/>
+      <c r="G28" s="188"/>
+      <c r="H28" s="188">
         <f>SUM(AU6:AW6,AU18:AW19,AU35:AW36,AU52:AW53)</f>
         <v>2</v>
       </c>
-      <c r="I28" s="181"/>
-      <c r="J28" s="181"/>
-      <c r="K28" s="181">
+      <c r="I28" s="188"/>
+      <c r="J28" s="188"/>
+      <c r="K28" s="188">
         <f>SUM(AX6:AZ6,AX18:AZ19,AX35:AZ36,AX52:AZ53)</f>
         <v>27</v>
       </c>
-      <c r="L28" s="181"/>
-      <c r="M28" s="181"/>
-      <c r="N28" s="181">
+      <c r="L28" s="188"/>
+      <c r="M28" s="188"/>
+      <c r="N28" s="188">
         <f>SUM(BA6:BC6,BA18:BC19,BA35:BC36,BA52:BC53)</f>
         <v>33</v>
       </c>
-      <c r="O28" s="181"/>
-      <c r="P28" s="181"/>
-      <c r="Q28" s="182">
+      <c r="O28" s="188"/>
+      <c r="P28" s="188"/>
+      <c r="Q28" s="187">
         <f>SUM(BD6:BF6,BD18:BF19,BD35:BF36,BD52:BF53)</f>
         <v>20</v>
       </c>
-      <c r="R28" s="182"/>
-      <c r="S28" s="182"/>
-      <c r="T28" s="181">
+      <c r="R28" s="187"/>
+      <c r="S28" s="187"/>
+      <c r="T28" s="188">
         <f t="shared" ref="T28" si="34">SUM(B28:S29)</f>
         <v>96</v>
       </c>
-      <c r="U28" s="177"/>
+      <c r="U28" s="196"/>
       <c r="BG28" s="158">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A29" s="183"/>
-      <c r="B29" s="181"/>
-      <c r="C29" s="181"/>
-      <c r="D29" s="181"/>
-      <c r="E29" s="181"/>
-      <c r="F29" s="181"/>
-      <c r="G29" s="181"/>
-      <c r="H29" s="181"/>
-      <c r="I29" s="181"/>
-      <c r="J29" s="181"/>
-      <c r="K29" s="181"/>
-      <c r="L29" s="181"/>
-      <c r="M29" s="181"/>
-      <c r="N29" s="181"/>
-      <c r="O29" s="181"/>
-      <c r="P29" s="181"/>
-      <c r="Q29" s="182"/>
-      <c r="R29" s="182"/>
-      <c r="S29" s="182"/>
-      <c r="T29" s="181"/>
-      <c r="U29" s="177"/>
+      <c r="A29" s="186"/>
+      <c r="B29" s="188"/>
+      <c r="C29" s="188"/>
+      <c r="D29" s="188"/>
+      <c r="E29" s="188"/>
+      <c r="F29" s="188"/>
+      <c r="G29" s="188"/>
+      <c r="H29" s="188"/>
+      <c r="I29" s="188"/>
+      <c r="J29" s="188"/>
+      <c r="K29" s="188"/>
+      <c r="L29" s="188"/>
+      <c r="M29" s="188"/>
+      <c r="N29" s="188"/>
+      <c r="O29" s="188"/>
+      <c r="P29" s="188"/>
+      <c r="Q29" s="187"/>
+      <c r="R29" s="187"/>
+      <c r="S29" s="187"/>
+      <c r="T29" s="188"/>
+      <c r="U29" s="196"/>
       <c r="AA29" t="s">
         <v>124</v>
       </c>
       <c r="AB29" s="149" t="s">
         <v>127</v>
       </c>
-      <c r="AC29" s="192" t="str">
+      <c r="AC29" s="179" t="str">
         <f>'3_PDC'!U6</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD29" s="193"/>
-      <c r="AE29" s="194"/>
-      <c r="AF29" s="192" t="str">
+      <c r="AD29" s="180"/>
+      <c r="AE29" s="181"/>
+      <c r="AF29" s="179" t="str">
         <f>'3_PDC'!X6</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG29" s="193"/>
-      <c r="AH29" s="195"/>
-      <c r="AI29" s="188" t="str">
+      <c r="AG29" s="180"/>
+      <c r="AH29" s="182"/>
+      <c r="AI29" s="183" t="str">
         <f>'3_PDC'!AA6</f>
         <v>Totale</v>
       </c>
@@ -13309,50 +13310,50 @@
       </c>
     </row>
     <row r="30" spans="1:60" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="183" t="s">
+      <c r="A30" s="186" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="181">
+      <c r="B30" s="188">
         <f>SUM(AO7:AQ7,AO20:AQ21,AO37:AQ38,AO54:AQ55)</f>
         <v>15</v>
       </c>
-      <c r="C30" s="181"/>
-      <c r="D30" s="181"/>
-      <c r="E30" s="181">
+      <c r="C30" s="188"/>
+      <c r="D30" s="188"/>
+      <c r="E30" s="188">
         <f>SUM(AR7:AT7,AR20:AT21,AR37:AT38,AR54:AT55)</f>
         <v>4</v>
       </c>
-      <c r="F30" s="181"/>
-      <c r="G30" s="181"/>
-      <c r="H30" s="181">
+      <c r="F30" s="188"/>
+      <c r="G30" s="188"/>
+      <c r="H30" s="188">
         <f>SUM(AU7:AW7,AU20:AW21,AU37:AW38,AU54:AW55)</f>
         <v>0</v>
       </c>
-      <c r="I30" s="181"/>
-      <c r="J30" s="181"/>
-      <c r="K30" s="182">
+      <c r="I30" s="188"/>
+      <c r="J30" s="188"/>
+      <c r="K30" s="187">
         <f>SUM(AX7:AZ7,AX20:AZ21,AX37:AZ38,AX54:AZ55)</f>
         <v>31</v>
       </c>
-      <c r="L30" s="182"/>
-      <c r="M30" s="182"/>
-      <c r="N30" s="182">
+      <c r="L30" s="187"/>
+      <c r="M30" s="187"/>
+      <c r="N30" s="187">
         <f>SUM(BA7:BC7,BA20:BC21,BA37:BC38,BA54:BC55)</f>
         <v>35</v>
       </c>
-      <c r="O30" s="182"/>
-      <c r="P30" s="182"/>
-      <c r="Q30" s="181">
+      <c r="O30" s="187"/>
+      <c r="P30" s="187"/>
+      <c r="Q30" s="188">
         <f>SUM(BD7:BF7,BD20:BF21,BD37:BF38,BD54:BF55)</f>
         <v>18</v>
       </c>
-      <c r="R30" s="181"/>
-      <c r="S30" s="181"/>
-      <c r="T30" s="181">
+      <c r="R30" s="188"/>
+      <c r="S30" s="188"/>
+      <c r="T30" s="188">
         <f t="shared" ref="T30" si="35">SUM(B30:S31)</f>
         <v>103</v>
       </c>
-      <c r="U30" s="177"/>
+      <c r="U30" s="196"/>
       <c r="AB30" s="150"/>
       <c r="AC30" s="26" t="str">
         <f>'3_PDC'!U7</f>
@@ -13378,7 +13379,7 @@
         <f>'3_PDC'!Z7</f>
         <v>Fase</v>
       </c>
-      <c r="AI30" s="189"/>
+      <c r="AI30" s="184"/>
       <c r="AK30">
         <f>SUM(AI31:AI44)</f>
         <v>373</v>
@@ -13389,27 +13390,27 @@
       </c>
     </row>
     <row r="31" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A31" s="183"/>
-      <c r="B31" s="181"/>
-      <c r="C31" s="181"/>
-      <c r="D31" s="181"/>
-      <c r="E31" s="181"/>
-      <c r="F31" s="181"/>
-      <c r="G31" s="181"/>
-      <c r="H31" s="181"/>
-      <c r="I31" s="181"/>
-      <c r="J31" s="181"/>
-      <c r="K31" s="182"/>
-      <c r="L31" s="182"/>
-      <c r="M31" s="182"/>
-      <c r="N31" s="182"/>
-      <c r="O31" s="182"/>
-      <c r="P31" s="182"/>
-      <c r="Q31" s="181"/>
-      <c r="R31" s="181"/>
-      <c r="S31" s="181"/>
-      <c r="T31" s="181"/>
-      <c r="U31" s="177"/>
+      <c r="A31" s="186"/>
+      <c r="B31" s="188"/>
+      <c r="C31" s="188"/>
+      <c r="D31" s="188"/>
+      <c r="E31" s="188"/>
+      <c r="F31" s="188"/>
+      <c r="G31" s="188"/>
+      <c r="H31" s="188"/>
+      <c r="I31" s="188"/>
+      <c r="J31" s="188"/>
+      <c r="K31" s="187"/>
+      <c r="L31" s="187"/>
+      <c r="M31" s="187"/>
+      <c r="N31" s="187"/>
+      <c r="O31" s="187"/>
+      <c r="P31" s="187"/>
+      <c r="Q31" s="188"/>
+      <c r="R31" s="188"/>
+      <c r="S31" s="188"/>
+      <c r="T31" s="188"/>
+      <c r="U31" s="196"/>
       <c r="AB31" s="31" t="str">
         <f>'3_PDC'!T8</f>
         <v>Begolo Marco</v>
@@ -13438,7 +13439,7 @@
         <f>'3_PDC'!Z8</f>
         <v>PDC 4.4</v>
       </c>
-      <c r="AI31" s="196">
+      <c r="AI31" s="185">
         <f>'3_PDC'!AA8</f>
         <v>52</v>
       </c>
@@ -13524,50 +13525,50 @@
       </c>
     </row>
     <row r="32" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A32" s="183" t="s">
+      <c r="A32" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="181">
+      <c r="B32" s="188">
         <f>SUM(AO8:AQ8,AO22:AQ23,AO39:AQ40,AO56:AQ57)</f>
         <v>9</v>
       </c>
-      <c r="C32" s="181"/>
-      <c r="D32" s="181"/>
-      <c r="E32" s="181">
+      <c r="C32" s="188"/>
+      <c r="D32" s="188"/>
+      <c r="E32" s="188">
         <f>SUM(AR8:AT8,AR22:AT23,AR39:AT40,AR56:AT57)</f>
         <v>11</v>
       </c>
-      <c r="F32" s="181"/>
-      <c r="G32" s="181"/>
-      <c r="H32" s="181">
+      <c r="F32" s="188"/>
+      <c r="G32" s="188"/>
+      <c r="H32" s="188">
         <f>SUM(AU8:AW8,AU22:AW23,AU39:AW40,AU56:AW57)</f>
         <v>2</v>
       </c>
-      <c r="I32" s="181"/>
-      <c r="J32" s="181"/>
-      <c r="K32" s="181">
+      <c r="I32" s="188"/>
+      <c r="J32" s="188"/>
+      <c r="K32" s="188">
         <f>SUM(AX8:AZ8,AX22:AZ23,AX39:AZ40,AX56:AZ57)</f>
         <v>20</v>
       </c>
-      <c r="L32" s="181"/>
-      <c r="M32" s="181"/>
-      <c r="N32" s="182">
+      <c r="L32" s="188"/>
+      <c r="M32" s="188"/>
+      <c r="N32" s="187">
         <f>SUM(BA8:BC8,BA22:BC23,BA39:BC40,BA56:BC57)</f>
         <v>37</v>
       </c>
-      <c r="O32" s="182"/>
-      <c r="P32" s="182"/>
-      <c r="Q32" s="181">
+      <c r="O32" s="187"/>
+      <c r="P32" s="187"/>
+      <c r="Q32" s="188">
         <f>SUM(BD8:BF8,BD22:BF23,BD39:BF40,BD56:BF57)</f>
         <v>23</v>
       </c>
-      <c r="R32" s="181"/>
-      <c r="S32" s="181"/>
-      <c r="T32" s="181">
+      <c r="R32" s="188"/>
+      <c r="S32" s="188"/>
+      <c r="T32" s="188">
         <f t="shared" ref="T32" si="51">SUM(B32:S33)</f>
         <v>102</v>
       </c>
-      <c r="U32" s="177"/>
+      <c r="U32" s="196"/>
       <c r="AB32" s="35">
         <f>'3_PDC'!T9</f>
         <v>0</v>
@@ -13596,7 +13597,7 @@
         <f>'3_PDC'!Z9</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI32" s="184"/>
+      <c r="AI32" s="177"/>
       <c r="AO32">
         <f>IF($AC32=AO$2,$AD32,0)</f>
         <v>0</v>
@@ -13675,27 +13676,27 @@
       </c>
     </row>
     <row r="33" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A33" s="183"/>
-      <c r="B33" s="181"/>
-      <c r="C33" s="181"/>
-      <c r="D33" s="181"/>
-      <c r="E33" s="181"/>
-      <c r="F33" s="181"/>
-      <c r="G33" s="181"/>
-      <c r="H33" s="181"/>
-      <c r="I33" s="181"/>
-      <c r="J33" s="181"/>
-      <c r="K33" s="181"/>
-      <c r="L33" s="181"/>
-      <c r="M33" s="181"/>
-      <c r="N33" s="182"/>
-      <c r="O33" s="182"/>
-      <c r="P33" s="182"/>
-      <c r="Q33" s="181"/>
-      <c r="R33" s="181"/>
-      <c r="S33" s="181"/>
-      <c r="T33" s="181"/>
-      <c r="U33" s="177"/>
+      <c r="A33" s="186"/>
+      <c r="B33" s="188"/>
+      <c r="C33" s="188"/>
+      <c r="D33" s="188"/>
+      <c r="E33" s="188"/>
+      <c r="F33" s="188"/>
+      <c r="G33" s="188"/>
+      <c r="H33" s="188"/>
+      <c r="I33" s="188"/>
+      <c r="J33" s="188"/>
+      <c r="K33" s="188"/>
+      <c r="L33" s="188"/>
+      <c r="M33" s="188"/>
+      <c r="N33" s="187"/>
+      <c r="O33" s="187"/>
+      <c r="P33" s="187"/>
+      <c r="Q33" s="188"/>
+      <c r="R33" s="188"/>
+      <c r="S33" s="188"/>
+      <c r="T33" s="188"/>
+      <c r="U33" s="196"/>
       <c r="AB33" s="31" t="str">
         <f>'3_PDC'!T10</f>
         <v>Facchin Gabriele</v>
@@ -13724,7 +13725,7 @@
         <f>'3_PDC'!Z10</f>
         <v>PDC 3.1</v>
       </c>
-      <c r="AI33" s="184">
+      <c r="AI33" s="177">
         <f>'3_PDC'!AA10</f>
         <v>52</v>
       </c>
@@ -13806,50 +13807,50 @@
       </c>
     </row>
     <row r="34" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A34" s="183" t="s">
+      <c r="A34" s="186" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="181">
+      <c r="B34" s="188">
         <f>SUM(AO9:AQ9,AO24:AQ25,AO41:AQ42,AO58:AQ59)</f>
         <v>6</v>
       </c>
-      <c r="C34" s="181"/>
-      <c r="D34" s="181"/>
-      <c r="E34" s="181">
+      <c r="C34" s="188"/>
+      <c r="D34" s="188"/>
+      <c r="E34" s="188">
         <f>SUM(AR9:AT9,AR24:AT25,AR41:AT42,AR58:AT59)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="181"/>
-      <c r="G34" s="181"/>
-      <c r="H34" s="181">
+      <c r="F34" s="188"/>
+      <c r="G34" s="188"/>
+      <c r="H34" s="188">
         <f>SUM(AU9:AW9,AU24:AW25,AU41:AW42,AU58:AW59)</f>
         <v>0</v>
       </c>
-      <c r="I34" s="181"/>
-      <c r="J34" s="181"/>
-      <c r="K34" s="182">
+      <c r="I34" s="188"/>
+      <c r="J34" s="188"/>
+      <c r="K34" s="187">
         <f>SUM(AX9:AZ9,AX24:AZ25,AX41:AZ42,AX58:AZ59)</f>
         <v>27</v>
       </c>
-      <c r="L34" s="182"/>
-      <c r="M34" s="182"/>
-      <c r="N34" s="182">
+      <c r="L34" s="187"/>
+      <c r="M34" s="187"/>
+      <c r="N34" s="187">
         <f>SUM(BA9:BC9,BA24:BC25,BA41:BC42,BA58:BC59)</f>
         <v>40</v>
       </c>
-      <c r="O34" s="182"/>
-      <c r="P34" s="182"/>
-      <c r="Q34" s="182">
+      <c r="O34" s="187"/>
+      <c r="P34" s="187"/>
+      <c r="Q34" s="187">
         <f>SUM(BD9:BF9,BD24:BF25,BD41:BF42,BD58:BF59)</f>
         <v>25</v>
       </c>
-      <c r="R34" s="182"/>
-      <c r="S34" s="182"/>
-      <c r="T34" s="181">
+      <c r="R34" s="187"/>
+      <c r="S34" s="187"/>
+      <c r="T34" s="188">
         <f t="shared" ref="T34" si="55">SUM(B34:S35)</f>
         <v>100</v>
       </c>
-      <c r="U34" s="177"/>
+      <c r="U34" s="196"/>
       <c r="AB34" s="31">
         <f>'3_PDC'!T11</f>
         <v>0</v>
@@ -13878,7 +13879,7 @@
         <f>'3_PDC'!Z11</f>
         <v>PDC 4.3</v>
       </c>
-      <c r="AI34" s="184"/>
+      <c r="AI34" s="177"/>
       <c r="AO34">
         <f t="shared" si="52"/>
         <v>0</v>
@@ -13957,27 +13958,27 @@
       </c>
     </row>
     <row r="35" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A35" s="183"/>
-      <c r="B35" s="181"/>
-      <c r="C35" s="181"/>
-      <c r="D35" s="181"/>
-      <c r="E35" s="181"/>
-      <c r="F35" s="181"/>
-      <c r="G35" s="181"/>
-      <c r="H35" s="181"/>
-      <c r="I35" s="181"/>
-      <c r="J35" s="181"/>
-      <c r="K35" s="182"/>
-      <c r="L35" s="182"/>
-      <c r="M35" s="182"/>
-      <c r="N35" s="182"/>
-      <c r="O35" s="182"/>
-      <c r="P35" s="182"/>
-      <c r="Q35" s="182"/>
-      <c r="R35" s="182"/>
-      <c r="S35" s="182"/>
-      <c r="T35" s="181"/>
-      <c r="U35" s="177"/>
+      <c r="A35" s="186"/>
+      <c r="B35" s="188"/>
+      <c r="C35" s="188"/>
+      <c r="D35" s="188"/>
+      <c r="E35" s="188"/>
+      <c r="F35" s="188"/>
+      <c r="G35" s="188"/>
+      <c r="H35" s="188"/>
+      <c r="I35" s="188"/>
+      <c r="J35" s="188"/>
+      <c r="K35" s="187"/>
+      <c r="L35" s="187"/>
+      <c r="M35" s="187"/>
+      <c r="N35" s="187"/>
+      <c r="O35" s="187"/>
+      <c r="P35" s="187"/>
+      <c r="Q35" s="187"/>
+      <c r="R35" s="187"/>
+      <c r="S35" s="187"/>
+      <c r="T35" s="188"/>
+      <c r="U35" s="196"/>
       <c r="AB35" s="47" t="str">
         <f>'3_PDC'!T12</f>
         <v>Cornaglia Alessando</v>
@@ -14006,7 +14007,7 @@
         <f>'3_PDC'!Z12</f>
         <v>PDC 4.4 e 5</v>
       </c>
-      <c r="AI35" s="184">
+      <c r="AI35" s="177">
         <f>'3_PDC'!AA12</f>
         <v>52</v>
       </c>
@@ -14095,50 +14096,50 @@
       </c>
     </row>
     <row r="36" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A36" s="183" t="s">
+      <c r="A36" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="181">
+      <c r="B36" s="188">
         <f>SUM(AO10:AQ10,AO26:AQ27,AO43:AQ44,AO60:AQ61)</f>
         <v>2</v>
       </c>
-      <c r="C36" s="181"/>
-      <c r="D36" s="181"/>
-      <c r="E36" s="181">
+      <c r="C36" s="188"/>
+      <c r="D36" s="188"/>
+      <c r="E36" s="188">
         <f>SUM(AR10:AT10,AR26:AT27,AR43:AT44,AR60:AT61)</f>
         <v>8</v>
       </c>
-      <c r="F36" s="181"/>
-      <c r="G36" s="181"/>
-      <c r="H36" s="181">
+      <c r="F36" s="188"/>
+      <c r="G36" s="188"/>
+      <c r="H36" s="188">
         <f>SUM(AU10:AW10,AU26:AW27,AU43:AW44,AU60:AW61)</f>
         <v>7</v>
       </c>
-      <c r="I36" s="181"/>
-      <c r="J36" s="181"/>
-      <c r="K36" s="182">
+      <c r="I36" s="188"/>
+      <c r="J36" s="188"/>
+      <c r="K36" s="187">
         <f>SUM(AX10:AZ10,AX26:AZ27,AX43:AZ44,AX60:AZ61)</f>
         <v>51</v>
       </c>
-      <c r="L36" s="182"/>
-      <c r="M36" s="182"/>
-      <c r="N36" s="181">
+      <c r="L36" s="187"/>
+      <c r="M36" s="187"/>
+      <c r="N36" s="188">
         <f>SUM(BA10:BC10,BA26:BC27,BA43:BC44,BA60:BC61)</f>
         <v>10</v>
       </c>
-      <c r="O36" s="181"/>
-      <c r="P36" s="181"/>
-      <c r="Q36" s="181">
+      <c r="O36" s="188"/>
+      <c r="P36" s="188"/>
+      <c r="Q36" s="188">
         <f>SUM(BD10:BF10,BD26:BF27,BD43:BF44,BD60:BF61)</f>
         <v>18</v>
       </c>
-      <c r="R36" s="181"/>
-      <c r="S36" s="181"/>
-      <c r="T36" s="181">
+      <c r="R36" s="188"/>
+      <c r="S36" s="188"/>
+      <c r="T36" s="188">
         <f t="shared" ref="T36" si="56">SUM(B36:S37)</f>
         <v>96</v>
       </c>
-      <c r="U36" s="177"/>
+      <c r="U36" s="196"/>
       <c r="AB36" s="35">
         <f>'3_PDC'!T13</f>
         <v>0</v>
@@ -14167,7 +14168,7 @@
         <f>'3_PDC'!Z13</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI36" s="184"/>
+      <c r="AI36" s="177"/>
       <c r="AK36">
         <f>SUM(BD31:BF44)</f>
         <v>100</v>
@@ -14250,27 +14251,27 @@
       </c>
     </row>
     <row r="37" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A37" s="183"/>
-      <c r="B37" s="181"/>
-      <c r="C37" s="181"/>
-      <c r="D37" s="181"/>
-      <c r="E37" s="181"/>
-      <c r="F37" s="181"/>
-      <c r="G37" s="181"/>
-      <c r="H37" s="181"/>
-      <c r="I37" s="181"/>
-      <c r="J37" s="181"/>
-      <c r="K37" s="182"/>
-      <c r="L37" s="182"/>
-      <c r="M37" s="182"/>
-      <c r="N37" s="181"/>
-      <c r="O37" s="181"/>
-      <c r="P37" s="181"/>
-      <c r="Q37" s="181"/>
-      <c r="R37" s="181"/>
-      <c r="S37" s="181"/>
-      <c r="T37" s="181"/>
-      <c r="U37" s="177"/>
+      <c r="A37" s="186"/>
+      <c r="B37" s="188"/>
+      <c r="C37" s="188"/>
+      <c r="D37" s="188"/>
+      <c r="E37" s="188"/>
+      <c r="F37" s="188"/>
+      <c r="G37" s="188"/>
+      <c r="H37" s="188"/>
+      <c r="I37" s="188"/>
+      <c r="J37" s="188"/>
+      <c r="K37" s="187"/>
+      <c r="L37" s="187"/>
+      <c r="M37" s="187"/>
+      <c r="N37" s="188"/>
+      <c r="O37" s="188"/>
+      <c r="P37" s="188"/>
+      <c r="Q37" s="188"/>
+      <c r="R37" s="188"/>
+      <c r="S37" s="188"/>
+      <c r="T37" s="188"/>
+      <c r="U37" s="196"/>
       <c r="AB37" s="31" t="str">
         <f>'3_PDC'!T14</f>
         <v>Dalla Pietà Massimo</v>
@@ -14299,7 +14300,7 @@
         <f>'3_PDC'!Z14</f>
         <v>PDC 4.3</v>
       </c>
-      <c r="AI37" s="184">
+      <c r="AI37" s="177">
         <f>'3_PDC'!AA14</f>
         <v>57</v>
       </c>
@@ -14381,50 +14382,50 @@
       </c>
     </row>
     <row r="38" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A38" s="180" t="s">
+      <c r="A38" s="195" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="181">
+      <c r="B38" s="188">
         <f>SUM(B24:D37)</f>
         <v>59</v>
       </c>
-      <c r="C38" s="181"/>
-      <c r="D38" s="181"/>
-      <c r="E38" s="181">
+      <c r="C38" s="188"/>
+      <c r="D38" s="188"/>
+      <c r="E38" s="188">
         <f t="shared" ref="E38" si="57">SUM(E24:G37)</f>
         <v>49</v>
       </c>
-      <c r="F38" s="181"/>
-      <c r="G38" s="181"/>
-      <c r="H38" s="181">
+      <c r="F38" s="188"/>
+      <c r="G38" s="188"/>
+      <c r="H38" s="188">
         <f>SUM(H24:J37)</f>
         <v>20</v>
       </c>
-      <c r="I38" s="181"/>
-      <c r="J38" s="181"/>
-      <c r="K38" s="181">
+      <c r="I38" s="188"/>
+      <c r="J38" s="188"/>
+      <c r="K38" s="188">
         <f t="shared" ref="K38" si="58">SUM(K24:M37)</f>
         <v>199</v>
       </c>
-      <c r="L38" s="181"/>
-      <c r="M38" s="181"/>
-      <c r="N38" s="181">
+      <c r="L38" s="188"/>
+      <c r="M38" s="188"/>
+      <c r="N38" s="188">
         <f t="shared" ref="N38" si="59">SUM(N24:P37)</f>
         <v>243</v>
       </c>
-      <c r="O38" s="181"/>
-      <c r="P38" s="181"/>
-      <c r="Q38" s="181">
+      <c r="O38" s="188"/>
+      <c r="P38" s="188"/>
+      <c r="Q38" s="188">
         <f>SUM(Q24:S37)</f>
         <v>120</v>
       </c>
-      <c r="R38" s="181"/>
-      <c r="S38" s="181"/>
+      <c r="R38" s="188"/>
+      <c r="S38" s="188"/>
       <c r="T38" s="199">
         <f>SUM(B38:S39)</f>
         <v>690</v>
       </c>
-      <c r="U38" s="177"/>
+      <c r="U38" s="196"/>
       <c r="AB38" s="31">
         <f>'3_PDC'!T15</f>
         <v>0</v>
@@ -14453,7 +14454,7 @@
         <f>'3_PDC'!Z15</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI38" s="184"/>
+      <c r="AI38" s="177"/>
       <c r="AO38">
         <f t="shared" si="52"/>
         <v>0</v>
@@ -14532,27 +14533,27 @@
       </c>
     </row>
     <row r="39" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A39" s="180"/>
-      <c r="B39" s="181"/>
-      <c r="C39" s="181"/>
-      <c r="D39" s="181"/>
-      <c r="E39" s="181"/>
-      <c r="F39" s="181"/>
-      <c r="G39" s="181"/>
-      <c r="H39" s="181"/>
-      <c r="I39" s="181"/>
-      <c r="J39" s="181"/>
-      <c r="K39" s="181"/>
-      <c r="L39" s="181"/>
-      <c r="M39" s="181"/>
-      <c r="N39" s="181"/>
-      <c r="O39" s="181"/>
-      <c r="P39" s="181"/>
-      <c r="Q39" s="181"/>
-      <c r="R39" s="181"/>
-      <c r="S39" s="181"/>
+      <c r="A39" s="195"/>
+      <c r="B39" s="188"/>
+      <c r="C39" s="188"/>
+      <c r="D39" s="188"/>
+      <c r="E39" s="188"/>
+      <c r="F39" s="188"/>
+      <c r="G39" s="188"/>
+      <c r="H39" s="188"/>
+      <c r="I39" s="188"/>
+      <c r="J39" s="188"/>
+      <c r="K39" s="188"/>
+      <c r="L39" s="188"/>
+      <c r="M39" s="188"/>
+      <c r="N39" s="188"/>
+      <c r="O39" s="188"/>
+      <c r="P39" s="188"/>
+      <c r="Q39" s="188"/>
+      <c r="R39" s="188"/>
+      <c r="S39" s="188"/>
       <c r="T39" s="199"/>
-      <c r="U39" s="177"/>
+      <c r="U39" s="196"/>
       <c r="AB39" s="47" t="str">
         <f>'3_PDC'!T16</f>
         <v>Braghetto Lorenzo</v>
@@ -14581,7 +14582,7 @@
         <f>'3_PDC'!Z16</f>
         <v>PDC 4.4</v>
       </c>
-      <c r="AI39" s="184">
+      <c r="AI39" s="177">
         <f>'3_PDC'!AA16</f>
         <v>54</v>
       </c>
@@ -14692,7 +14693,7 @@
         <f>'3_PDC'!Z17</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI40" s="184"/>
+      <c r="AI40" s="177"/>
       <c r="AO40">
         <f t="shared" si="52"/>
         <v>0</v>
@@ -14800,7 +14801,7 @@
         <f>'3_PDC'!Z18</f>
         <v>PDC 6</v>
       </c>
-      <c r="AI41" s="184">
+      <c r="AI41" s="177">
         <f>'3_PDC'!AA18</f>
         <v>54</v>
       </c>
@@ -14911,7 +14912,7 @@
         <f>'3_PDC'!Z19</f>
         <v>PDC 3.2, 5 e 7</v>
       </c>
-      <c r="AI42" s="184"/>
+      <c r="AI42" s="177"/>
       <c r="AO42">
         <f t="shared" si="52"/>
         <v>0</v>
@@ -15019,7 +15020,7 @@
         <f>'3_PDC'!Z20</f>
         <v>PDC 4.3</v>
       </c>
-      <c r="AI43" s="184">
+      <c r="AI43" s="177">
         <f>'3_PDC'!AA20</f>
         <v>52</v>
       </c>
@@ -15130,7 +15131,7 @@
         <f>'3_PDC'!Z21</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI44" s="198"/>
+      <c r="AI44" s="178"/>
       <c r="AO44">
         <f t="shared" si="52"/>
         <v>0</v>
@@ -15223,19 +15224,19 @@
       <c r="AB46" s="149" t="s">
         <v>128</v>
       </c>
-      <c r="AC46" s="192" t="str">
+      <c r="AC46" s="179" t="str">
         <f>'4_VV'!U3</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD46" s="193"/>
-      <c r="AE46" s="194"/>
-      <c r="AF46" s="192" t="str">
+      <c r="AD46" s="180"/>
+      <c r="AE46" s="181"/>
+      <c r="AF46" s="179" t="str">
         <f>'4_VV'!X3</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG46" s="193"/>
-      <c r="AH46" s="195"/>
-      <c r="AI46" s="188" t="str">
+      <c r="AG46" s="180"/>
+      <c r="AH46" s="182"/>
+      <c r="AI46" s="183" t="str">
         <f>'4_VV'!AA3</f>
         <v>Totale</v>
       </c>
@@ -15275,7 +15276,7 @@
         <f>'4_VV'!Z4</f>
         <v>Fase</v>
       </c>
-      <c r="AI47" s="189"/>
+      <c r="AI47" s="184"/>
       <c r="BG47" s="158">
         <f t="shared" si="13"/>
         <v>0</v>
@@ -15311,7 +15312,7 @@
         <f>'4_VV'!Z5</f>
         <v>VV 3.2</v>
       </c>
-      <c r="AI48" s="196">
+      <c r="AI48" s="185">
         <f>'4_VV'!AA5</f>
         <v>18</v>
       </c>
@@ -15425,7 +15426,7 @@
         <f>'4_VV'!Z6</f>
         <v>0</v>
       </c>
-      <c r="AI49" s="184"/>
+      <c r="AI49" s="177"/>
       <c r="AO49">
         <f>IF($AC49=AO$2,$AD49,0)</f>
         <v>0</v>
@@ -15532,7 +15533,7 @@
         <f>'4_VV'!Z7</f>
         <v>VV 3.2</v>
       </c>
-      <c r="AI50" s="184">
+      <c r="AI50" s="177">
         <f>'4_VV'!AA7</f>
         <v>18</v>
       </c>
@@ -15661,7 +15662,7 @@
         <f>'4_VV'!Z8</f>
         <v>VV 3.2</v>
       </c>
-      <c r="AI51" s="184"/>
+      <c r="AI51" s="177"/>
       <c r="AO51">
         <f t="shared" si="75"/>
         <v>0</v>
@@ -15782,7 +15783,7 @@
         <f>'4_VV'!Z9</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI52" s="184">
+      <c r="AI52" s="177">
         <f>'4_VV'!AA9</f>
         <v>18</v>
       </c>
@@ -15906,7 +15907,7 @@
         <f>'4_VV'!Z10</f>
         <v>0</v>
       </c>
-      <c r="AI53" s="184"/>
+      <c r="AI53" s="177"/>
       <c r="AO53">
         <f t="shared" si="75"/>
         <v>0</v>
@@ -16027,7 +16028,7 @@
         <f>'4_VV'!Z11</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI54" s="184">
+      <c r="AI54" s="177">
         <f>'4_VV'!AA11</f>
         <v>18</v>
       </c>
@@ -16151,7 +16152,7 @@
         <f>'4_VV'!Z12</f>
         <v>0</v>
       </c>
-      <c r="AI55" s="184"/>
+      <c r="AI55" s="177"/>
       <c r="AO55">
         <f t="shared" si="75"/>
         <v>0</v>
@@ -16272,7 +16273,7 @@
         <f>'4_VV'!Z13</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI56" s="184">
+      <c r="AI56" s="177">
         <f>'4_VV'!AA13</f>
         <v>18</v>
       </c>
@@ -16396,7 +16397,7 @@
         <f>'4_VV'!Z14</f>
         <v>0</v>
       </c>
-      <c r="AI57" s="184"/>
+      <c r="AI57" s="177"/>
       <c r="AO57">
         <f t="shared" si="75"/>
         <v>0</v>
@@ -16514,7 +16515,7 @@
         <f>'4_VV'!Z15</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI58" s="184">
+      <c r="AI58" s="177">
         <f>'4_VV'!AA15</f>
         <v>18</v>
       </c>
@@ -16624,7 +16625,7 @@
         <f>'4_VV'!Z16</f>
         <v>0</v>
       </c>
-      <c r="AI59" s="184"/>
+      <c r="AI59" s="177"/>
       <c r="AO59">
         <f t="shared" si="75"/>
         <v>0</v>
@@ -16731,7 +16732,7 @@
         <f>'4_VV'!Z17</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI60" s="184">
+      <c r="AI60" s="177">
         <f>'4_VV'!AA17</f>
         <v>16</v>
       </c>
@@ -16841,7 +16842,7 @@
         <f>'4_VV'!Z18</f>
         <v>0</v>
       </c>
-      <c r="AI61" s="198"/>
+      <c r="AI61" s="178"/>
       <c r="AO61">
         <f t="shared" si="75"/>
         <v>0</v>
@@ -16921,18 +16922,82 @@
     </row>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AC12:AE12"/>
-    <mergeCell ref="AF12:AH12"/>
-    <mergeCell ref="AI12:AK12"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="AI56:AI57"/>
+    <mergeCell ref="AI58:AI59"/>
+    <mergeCell ref="AI60:AI61"/>
+    <mergeCell ref="AC46:AE46"/>
+    <mergeCell ref="AF46:AH46"/>
+    <mergeCell ref="AI46:AI47"/>
+    <mergeCell ref="AI48:AI49"/>
+    <mergeCell ref="AI50:AI51"/>
+    <mergeCell ref="AI52:AI53"/>
+    <mergeCell ref="AI39:AI40"/>
+    <mergeCell ref="AI41:AI42"/>
+    <mergeCell ref="AI43:AI44"/>
+    <mergeCell ref="Q36:S37"/>
+    <mergeCell ref="T36:T37"/>
+    <mergeCell ref="U36:U37"/>
+    <mergeCell ref="AI37:AI38"/>
+    <mergeCell ref="AI35:AI36"/>
+    <mergeCell ref="AI54:AI55"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:D39"/>
+    <mergeCell ref="E38:G39"/>
+    <mergeCell ref="H38:J39"/>
+    <mergeCell ref="K38:M39"/>
+    <mergeCell ref="N38:P39"/>
+    <mergeCell ref="Q34:S35"/>
+    <mergeCell ref="T34:T35"/>
+    <mergeCell ref="U34:U35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:D37"/>
+    <mergeCell ref="E36:G37"/>
+    <mergeCell ref="H36:J37"/>
+    <mergeCell ref="K36:M37"/>
+    <mergeCell ref="N36:P37"/>
+    <mergeCell ref="Q38:S39"/>
+    <mergeCell ref="T38:T39"/>
+    <mergeCell ref="U38:U39"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:D35"/>
+    <mergeCell ref="E34:G35"/>
+    <mergeCell ref="H34:J35"/>
+    <mergeCell ref="K34:M35"/>
+    <mergeCell ref="N34:P35"/>
+    <mergeCell ref="B24:D25"/>
+    <mergeCell ref="E24:G25"/>
+    <mergeCell ref="H24:J25"/>
+    <mergeCell ref="K24:M25"/>
+    <mergeCell ref="N24:P25"/>
+    <mergeCell ref="AC29:AE29"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:D33"/>
+    <mergeCell ref="E32:G33"/>
+    <mergeCell ref="H32:J33"/>
+    <mergeCell ref="K32:M33"/>
+    <mergeCell ref="N32:P33"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:D31"/>
+    <mergeCell ref="E30:G31"/>
+    <mergeCell ref="H30:J31"/>
+    <mergeCell ref="K30:M31"/>
+    <mergeCell ref="N30:P31"/>
+    <mergeCell ref="AF29:AH29"/>
+    <mergeCell ref="AI29:AI30"/>
+    <mergeCell ref="Q30:S31"/>
+    <mergeCell ref="T30:T31"/>
+    <mergeCell ref="U30:U31"/>
+    <mergeCell ref="AI31:AI32"/>
+    <mergeCell ref="Q26:S27"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="Q32:S33"/>
+    <mergeCell ref="T32:T33"/>
+    <mergeCell ref="U32:U33"/>
+    <mergeCell ref="AI33:AI34"/>
+    <mergeCell ref="Q28:S29"/>
+    <mergeCell ref="T28:T29"/>
+    <mergeCell ref="U28:U29"/>
     <mergeCell ref="AL12:AL13"/>
     <mergeCell ref="AL14:AL15"/>
     <mergeCell ref="AL16:AL17"/>
@@ -16957,82 +17022,18 @@
     <mergeCell ref="K26:M27"/>
     <mergeCell ref="N26:P27"/>
     <mergeCell ref="A24:A25"/>
-    <mergeCell ref="AF29:AH29"/>
-    <mergeCell ref="AI29:AI30"/>
-    <mergeCell ref="Q30:S31"/>
-    <mergeCell ref="T30:T31"/>
-    <mergeCell ref="U30:U31"/>
-    <mergeCell ref="AI31:AI32"/>
-    <mergeCell ref="Q26:S27"/>
-    <mergeCell ref="T26:T27"/>
-    <mergeCell ref="U26:U27"/>
-    <mergeCell ref="Q32:S33"/>
-    <mergeCell ref="T32:T33"/>
-    <mergeCell ref="U32:U33"/>
-    <mergeCell ref="AI33:AI34"/>
-    <mergeCell ref="Q28:S29"/>
-    <mergeCell ref="T28:T29"/>
-    <mergeCell ref="U28:U29"/>
-    <mergeCell ref="B24:D25"/>
-    <mergeCell ref="E24:G25"/>
-    <mergeCell ref="H24:J25"/>
-    <mergeCell ref="K24:M25"/>
-    <mergeCell ref="N24:P25"/>
-    <mergeCell ref="AC29:AE29"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:D33"/>
-    <mergeCell ref="E32:G33"/>
-    <mergeCell ref="H32:J33"/>
-    <mergeCell ref="K32:M33"/>
-    <mergeCell ref="N32:P33"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:D31"/>
-    <mergeCell ref="E30:G31"/>
-    <mergeCell ref="H30:J31"/>
-    <mergeCell ref="K30:M31"/>
-    <mergeCell ref="N30:P31"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:D39"/>
-    <mergeCell ref="E38:G39"/>
-    <mergeCell ref="H38:J39"/>
-    <mergeCell ref="K38:M39"/>
-    <mergeCell ref="N38:P39"/>
-    <mergeCell ref="Q34:S35"/>
-    <mergeCell ref="T34:T35"/>
-    <mergeCell ref="U34:U35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:D37"/>
-    <mergeCell ref="E36:G37"/>
-    <mergeCell ref="H36:J37"/>
-    <mergeCell ref="K36:M37"/>
-    <mergeCell ref="N36:P37"/>
-    <mergeCell ref="Q38:S39"/>
-    <mergeCell ref="T38:T39"/>
-    <mergeCell ref="U38:U39"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:D35"/>
-    <mergeCell ref="E34:G35"/>
-    <mergeCell ref="H34:J35"/>
-    <mergeCell ref="K34:M35"/>
-    <mergeCell ref="N34:P35"/>
-    <mergeCell ref="AI39:AI40"/>
-    <mergeCell ref="AI41:AI42"/>
-    <mergeCell ref="AI43:AI44"/>
-    <mergeCell ref="Q36:S37"/>
-    <mergeCell ref="T36:T37"/>
-    <mergeCell ref="U36:U37"/>
-    <mergeCell ref="AI37:AI38"/>
-    <mergeCell ref="AI35:AI36"/>
-    <mergeCell ref="AI54:AI55"/>
-    <mergeCell ref="AI56:AI57"/>
-    <mergeCell ref="AI58:AI59"/>
-    <mergeCell ref="AI60:AI61"/>
-    <mergeCell ref="AC46:AE46"/>
-    <mergeCell ref="AF46:AH46"/>
-    <mergeCell ref="AI46:AI47"/>
-    <mergeCell ref="AI48:AI49"/>
-    <mergeCell ref="AI50:AI51"/>
-    <mergeCell ref="AI52:AI53"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AC12:AE12"/>
+    <mergeCell ref="AF12:AH12"/>
+    <mergeCell ref="AI12:AK12"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
   </mergeCells>
   <conditionalFormatting sqref="AB14:AL27">
     <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
@@ -17166,20 +17167,20 @@
       <c r="N2" s="155">
         <v>30</v>
       </c>
-      <c r="O2" s="188" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="185" t="s">
+      <c r="O2" s="183" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="189" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="186"/>
-      <c r="R2" s="187"/>
-      <c r="S2" s="185" t="s">
+      <c r="Q2" s="190"/>
+      <c r="R2" s="191"/>
+      <c r="S2" s="189" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="186"/>
-      <c r="U2" s="187"/>
-      <c r="V2" s="188" t="s">
+      <c r="T2" s="190"/>
+      <c r="U2" s="191"/>
+      <c r="V2" s="183" t="s">
         <v>14</v>
       </c>
     </row>
@@ -17241,7 +17242,7 @@
       <c r="U3" s="106" t="s">
         <v>39</v>
       </c>
-      <c r="V3" s="189"/>
+      <c r="V3" s="184"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
@@ -18459,29 +18460,29 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O9" s="192"/>
-      <c r="P9" s="193"/>
-      <c r="Q9" s="193"/>
-      <c r="R9" s="194"/>
-      <c r="U9" s="188" t="s">
-        <v>0</v>
-      </c>
-      <c r="V9" s="192" t="s">
+      <c r="O9" s="179"/>
+      <c r="P9" s="180"/>
+      <c r="Q9" s="180"/>
+      <c r="R9" s="181"/>
+      <c r="U9" s="183" t="s">
+        <v>0</v>
+      </c>
+      <c r="V9" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="W9" s="193"/>
-      <c r="X9" s="194"/>
-      <c r="Y9" s="192" t="s">
+      <c r="W9" s="180"/>
+      <c r="X9" s="181"/>
+      <c r="Y9" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="Z9" s="193"/>
-      <c r="AA9" s="194"/>
-      <c r="AB9" s="192" t="s">
+      <c r="Z9" s="180"/>
+      <c r="AA9" s="181"/>
+      <c r="AB9" s="179" t="s">
         <v>114</v>
       </c>
-      <c r="AC9" s="193"/>
-      <c r="AD9" s="195"/>
-      <c r="AE9" s="188" t="s">
+      <c r="AC9" s="180"/>
+      <c r="AD9" s="182"/>
+      <c r="AE9" s="183" t="s">
         <v>14</v>
       </c>
     </row>
@@ -18520,11 +18521,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O10" s="201"/>
+      <c r="O10" s="206"/>
       <c r="P10" s="93"/>
       <c r="Q10" s="93"/>
       <c r="R10" s="94"/>
-      <c r="U10" s="189"/>
+      <c r="U10" s="184"/>
       <c r="V10" s="26" t="s">
         <v>26</v>
       </c>
@@ -18552,7 +18553,7 @@
       <c r="AD10" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="AE10" s="189"/>
+      <c r="AE10" s="184"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -18627,7 +18628,7 @@
       <c r="AD11" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="AE11" s="196">
+      <c r="AE11" s="185">
         <f>SUM(Z11:Z12,AC11:AC12,W11:W12)</f>
         <v>26</v>
       </c>
@@ -18685,7 +18686,7 @@
       <c r="AB12" s="36"/>
       <c r="AC12" s="37"/>
       <c r="AD12" s="139"/>
-      <c r="AE12" s="184"/>
+      <c r="AE12" s="177"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
@@ -18756,7 +18757,7 @@
       <c r="AD13" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="AE13" s="184">
+      <c r="AE13" s="177">
         <f t="shared" ref="AE13" si="7">SUM(Z13:Z14,AC13:AC14,W13:W14)</f>
         <v>27</v>
       </c>
@@ -18820,7 +18821,7 @@
       <c r="AB14" s="32"/>
       <c r="AC14" s="33"/>
       <c r="AD14" s="7"/>
-      <c r="AE14" s="184"/>
+      <c r="AE14" s="177"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
@@ -18895,7 +18896,7 @@
       <c r="AD15" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="AE15" s="184">
+      <c r="AE15" s="177">
         <f t="shared" ref="AE15" si="8">SUM(Z15:Z16,AC15:AC16,W15:W16)</f>
         <v>26</v>
       </c>
@@ -18965,7 +18966,7 @@
       <c r="AD16" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="AE16" s="184"/>
+      <c r="AE16" s="177"/>
     </row>
     <row r="17" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
@@ -19040,7 +19041,7 @@
       <c r="AD17" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="AE17" s="184">
+      <c r="AE17" s="177">
         <f t="shared" ref="AE17" si="9">SUM(Z17:Z18,AC17:AC18,W17:W18)</f>
         <v>28</v>
       </c>
@@ -19106,7 +19107,7 @@
       <c r="AD18" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="AE18" s="184"/>
+      <c r="AE18" s="177"/>
     </row>
     <row r="19" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U19" s="47" t="s">
@@ -19139,7 +19140,7 @@
       <c r="AD19" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="AE19" s="184">
+      <c r="AE19" s="177">
         <f t="shared" ref="AE19" si="10">SUM(Z19:Z20,AC19:AC20,W19:W20)</f>
         <v>30</v>
       </c>
@@ -19186,7 +19187,7 @@
         <v>2</v>
       </c>
       <c r="AD20" s="39"/>
-      <c r="AE20" s="184"/>
+      <c r="AE20" s="177"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="U21" s="31" t="s">
@@ -19219,7 +19220,7 @@
       <c r="AD21" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="AE21" s="184">
+      <c r="AE21" s="177">
         <f t="shared" ref="AE21" si="11">SUM(Z21:Z22,AC21:AC22,W21:W22)</f>
         <v>28</v>
       </c>
@@ -19236,7 +19237,7 @@
       <c r="AB22" s="32"/>
       <c r="AC22" s="33"/>
       <c r="AD22" s="7"/>
-      <c r="AE22" s="184"/>
+      <c r="AE22" s="177"/>
     </row>
     <row r="23" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O23" s="30"/>
@@ -19270,7 +19271,7 @@
       <c r="AD23" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="AE23" s="184">
+      <c r="AE23" s="177">
         <f t="shared" ref="AE23" si="12">SUM(Z23:Z24,AC23:AC24,W23:W24)</f>
         <v>28</v>
       </c>
@@ -19334,7 +19335,7 @@
       <c r="AD24" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="AE24" s="198"/>
+      <c r="AE24" s="178"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -19560,25 +19561,25 @@
       <c r="R28" s="155">
         <v>15</v>
       </c>
-      <c r="U28" s="202" t="s">
-        <v>0</v>
-      </c>
-      <c r="V28" s="185" t="s">
+      <c r="U28" s="204" t="s">
+        <v>0</v>
+      </c>
+      <c r="V28" s="189" t="s">
         <v>18</v>
       </c>
-      <c r="W28" s="190"/>
-      <c r="X28" s="191"/>
-      <c r="Y28" s="185" t="s">
+      <c r="W28" s="192"/>
+      <c r="X28" s="193"/>
+      <c r="Y28" s="189" t="s">
         <v>19</v>
       </c>
-      <c r="Z28" s="190"/>
-      <c r="AA28" s="191"/>
-      <c r="AB28" s="185" t="s">
+      <c r="Z28" s="192"/>
+      <c r="AA28" s="193"/>
+      <c r="AB28" s="189" t="s">
         <v>114</v>
       </c>
-      <c r="AC28" s="190"/>
-      <c r="AD28" s="191"/>
-      <c r="AE28" s="202" t="s">
+      <c r="AC28" s="192"/>
+      <c r="AD28" s="193"/>
+      <c r="AE28" s="204" t="s">
         <v>14</v>
       </c>
     </row>
@@ -19631,7 +19632,7 @@
       <c r="R29" s="155">
         <v>22</v>
       </c>
-      <c r="U29" s="203"/>
+      <c r="U29" s="205"/>
       <c r="V29" s="26" t="s">
         <v>26</v>
       </c>
@@ -19659,7 +19660,7 @@
       <c r="AD29" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="AE29" s="203"/>
+      <c r="AE29" s="205"/>
     </row>
     <row r="30" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
@@ -19743,7 +19744,7 @@
       <c r="AD30" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="AE30" s="206">
+      <c r="AE30" s="203">
         <f>SUM(Z30:Z31,AC30:AC31,W30:W31)</f>
         <v>27</v>
       </c>
@@ -19799,7 +19800,7 @@
       <c r="AB31" s="36"/>
       <c r="AC31" s="37"/>
       <c r="AD31" s="139"/>
-      <c r="AE31" s="196"/>
+      <c r="AE31" s="185"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -19870,7 +19871,7 @@
       <c r="AD32" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="AE32" s="204">
+      <c r="AE32" s="201">
         <f t="shared" ref="AE32" si="20">SUM(Z32:Z33,AC32:AC33,W32:W33)</f>
         <v>27</v>
       </c>
@@ -19926,7 +19927,7 @@
       <c r="AB33" s="32"/>
       <c r="AC33" s="33"/>
       <c r="AD33" s="7"/>
-      <c r="AE33" s="196"/>
+      <c r="AE33" s="185"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
@@ -19997,7 +19998,7 @@
       <c r="AD34" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="AE34" s="204">
+      <c r="AE34" s="201">
         <f t="shared" ref="AE34" si="21">SUM(Z34:Z35,AC34:AC35,W34:W35)</f>
         <v>29</v>
       </c>
@@ -20063,7 +20064,7 @@
       <c r="AD35" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="AE35" s="196"/>
+      <c r="AE35" s="185"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
@@ -20130,7 +20131,7 @@
       <c r="AD36" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="AE36" s="204">
+      <c r="AE36" s="201">
         <f t="shared" ref="AE36" si="22">SUM(Z36:Z37,AC36:AC37,W36:W37)</f>
         <v>27</v>
       </c>
@@ -20196,7 +20197,7 @@
       <c r="AD37" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="AE37" s="196"/>
+      <c r="AE37" s="185"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
@@ -20267,7 +20268,7 @@
       <c r="AD38" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="AE38" s="204">
+      <c r="AE38" s="201">
         <f t="shared" ref="AE38" si="23">SUM(Z38:Z39,AC38:AC39,W38:W39)</f>
         <v>27</v>
       </c>
@@ -20327,7 +20328,7 @@
       <c r="AB39" s="36"/>
       <c r="AC39" s="37"/>
       <c r="AD39" s="39"/>
-      <c r="AE39" s="196"/>
+      <c r="AE39" s="185"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
@@ -20398,7 +20399,7 @@
       <c r="AD40" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="AE40" s="204">
+      <c r="AE40" s="201">
         <f t="shared" ref="AE40" si="24">SUM(Z40:Z41,AC40:AC41,W40:W41)</f>
         <v>27</v>
       </c>
@@ -20448,7 +20449,7 @@
       <c r="AB41" s="32"/>
       <c r="AC41" s="33"/>
       <c r="AD41" s="7"/>
-      <c r="AE41" s="196"/>
+      <c r="AE41" s="185"/>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="U42" s="47" t="s">
@@ -20481,7 +20482,7 @@
       <c r="AD42" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="AE42" s="204">
+      <c r="AE42" s="201">
         <f t="shared" ref="AE42" si="25">SUM(Z42:Z43,AC42:AC43,W42:W43)</f>
         <v>29</v>
       </c>
@@ -20509,7 +20510,7 @@
       <c r="AD43" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="AE43" s="205"/>
+      <c r="AE43" s="202"/>
     </row>
     <row r="49" spans="35:35" x14ac:dyDescent="0.25">
       <c r="AI49" t="s">
@@ -20518,18 +20519,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AE40:AE41"/>
-    <mergeCell ref="AE42:AE43"/>
-    <mergeCell ref="AE30:AE31"/>
-    <mergeCell ref="AE32:AE33"/>
-    <mergeCell ref="AE34:AE35"/>
-    <mergeCell ref="AE36:AE37"/>
-    <mergeCell ref="AE38:AE39"/>
-    <mergeCell ref="U28:U29"/>
-    <mergeCell ref="V28:X28"/>
-    <mergeCell ref="Y28:AA28"/>
-    <mergeCell ref="AB28:AD28"/>
-    <mergeCell ref="AE28:AE29"/>
+    <mergeCell ref="AB9:AD9"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="Y9:AA9"/>
     <mergeCell ref="AE21:AE22"/>
     <mergeCell ref="AE23:AE24"/>
     <mergeCell ref="AE9:AE10"/>
@@ -20538,12 +20533,18 @@
     <mergeCell ref="AE15:AE16"/>
     <mergeCell ref="AE17:AE18"/>
     <mergeCell ref="AE19:AE20"/>
-    <mergeCell ref="AB9:AD9"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="Y9:AA9"/>
+    <mergeCell ref="U28:U29"/>
+    <mergeCell ref="V28:X28"/>
+    <mergeCell ref="Y28:AA28"/>
+    <mergeCell ref="AB28:AD28"/>
+    <mergeCell ref="AE28:AE29"/>
+    <mergeCell ref="AE40:AE41"/>
+    <mergeCell ref="AE42:AE43"/>
+    <mergeCell ref="AE30:AE31"/>
+    <mergeCell ref="AE32:AE33"/>
+    <mergeCell ref="AE34:AE35"/>
+    <mergeCell ref="AE36:AE37"/>
+    <mergeCell ref="AE38:AE39"/>
   </mergeCells>
   <conditionalFormatting sqref="Z26">
     <cfRule type="cellIs" dxfId="15" priority="15" operator="notEqual">
@@ -20918,20 +20919,20 @@
       <c r="R6" s="155">
         <v>15</v>
       </c>
-      <c r="T6" s="188" t="s">
-        <v>0</v>
-      </c>
-      <c r="U6" s="192" t="s">
+      <c r="T6" s="183" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="V6" s="193"/>
-      <c r="W6" s="194"/>
-      <c r="X6" s="192" t="s">
+      <c r="V6" s="180"/>
+      <c r="W6" s="181"/>
+      <c r="X6" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="Y6" s="193"/>
-      <c r="Z6" s="195"/>
-      <c r="AA6" s="188" t="s">
+      <c r="Y6" s="180"/>
+      <c r="Z6" s="182"/>
+      <c r="AA6" s="183" t="s">
         <v>14</v>
       </c>
     </row>
@@ -20984,7 +20985,7 @@
         <f>SUM(Q2:Q6)</f>
         <v>6982</v>
       </c>
-      <c r="T7" s="189"/>
+      <c r="T7" s="184"/>
       <c r="U7" s="26" t="s">
         <v>26</v>
       </c>
@@ -21003,7 +21004,7 @@
       <c r="Z7" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="AA7" s="189"/>
+      <c r="AA7" s="184"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -21065,7 +21066,7 @@
       <c r="Z8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AA8" s="196">
+      <c r="AA8" s="185">
         <f>SUM(V8:V9,Y8:Y9)</f>
         <v>52</v>
       </c>
@@ -21117,7 +21118,7 @@
       <c r="Z9" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="AA9" s="184"/>
+      <c r="AA9" s="177"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
@@ -21178,7 +21179,7 @@
       <c r="Z10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AA10" s="184">
+      <c r="AA10" s="177">
         <f t="shared" ref="AA10" si="7">SUM(V10:V11,Y10:Y11)</f>
         <v>52</v>
       </c>
@@ -21240,7 +21241,7 @@
       <c r="Z11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA11" s="184"/>
+      <c r="AA11" s="177"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
@@ -21300,7 +21301,7 @@
       <c r="Z12" s="79" t="s">
         <v>130</v>
       </c>
-      <c r="AA12" s="184">
+      <c r="AA12" s="177">
         <f t="shared" ref="AA12" si="8">SUM(V12:V13,Y12:Y13)</f>
         <v>52</v>
       </c>
@@ -21365,7 +21366,7 @@
       <c r="Z13" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="AA13" s="184"/>
+      <c r="AA13" s="177"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -21429,7 +21430,7 @@
       <c r="Z14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA14" s="184">
+      <c r="AA14" s="177">
         <f t="shared" ref="AA14" si="9">SUM(V14:V15,Y14:Y15)</f>
         <v>57</v>
       </c>
@@ -21490,7 +21491,7 @@
       <c r="Z15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AA15" s="184"/>
+      <c r="AA15" s="177"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
@@ -21554,7 +21555,7 @@
       <c r="Z16" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="AA16" s="184">
+      <c r="AA16" s="177">
         <f t="shared" ref="AA16" si="10">SUM(V16:V17,Y16:Y17)</f>
         <v>54</v>
       </c>
@@ -21619,7 +21620,7 @@
       <c r="Z17" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="AA17" s="184"/>
+      <c r="AA17" s="177"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
@@ -21679,7 +21680,7 @@
       <c r="Z18" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="AA18" s="184">
+      <c r="AA18" s="177">
         <f t="shared" ref="AA18" si="11">SUM(V18:V19,Y18:Y19)</f>
         <v>54</v>
       </c>
@@ -21744,7 +21745,7 @@
       <c r="Z19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="AA19" s="184"/>
+      <c r="AA19" s="177"/>
     </row>
     <row r="20" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
@@ -21804,7 +21805,7 @@
       <c r="Z20" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="AA20" s="184">
+      <c r="AA20" s="177">
         <f t="shared" ref="AA20" si="12">SUM(V20:V21,Y20:Y21)</f>
         <v>52</v>
       </c>
@@ -21863,7 +21864,7 @@
       <c r="Z21" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="AA21" s="198"/>
+      <c r="AA21" s="178"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
@@ -22104,6 +22105,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AA10:AA11"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="X6:Z6"/>
+    <mergeCell ref="AA6:AA7"/>
+    <mergeCell ref="AA8:AA9"/>
     <mergeCell ref="AA20:AA21"/>
     <mergeCell ref="O12:O13"/>
     <mergeCell ref="P12:Q12"/>
@@ -22111,12 +22118,6 @@
     <mergeCell ref="AA14:AA15"/>
     <mergeCell ref="AA16:AA17"/>
     <mergeCell ref="AA18:AA19"/>
-    <mergeCell ref="AA10:AA11"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="X6:Z6"/>
-    <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="AA8:AA9"/>
   </mergeCells>
   <conditionalFormatting sqref="Y24">
     <cfRule type="cellIs" dxfId="7" priority="3" operator="notEqual">
@@ -22324,20 +22325,20 @@
       <c r="R3" s="155">
         <v>20</v>
       </c>
-      <c r="T3" s="188" t="s">
-        <v>0</v>
-      </c>
-      <c r="U3" s="192" t="s">
+      <c r="T3" s="183" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="V3" s="193"/>
-      <c r="W3" s="194"/>
-      <c r="X3" s="192" t="s">
+      <c r="V3" s="180"/>
+      <c r="W3" s="181"/>
+      <c r="X3" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="Y3" s="193"/>
-      <c r="Z3" s="195"/>
-      <c r="AA3" s="188" t="s">
+      <c r="Y3" s="180"/>
+      <c r="Z3" s="182"/>
+      <c r="AA3" s="183" t="s">
         <v>14</v>
       </c>
     </row>
@@ -22389,7 +22390,7 @@
       <c r="R4" s="155">
         <v>15</v>
       </c>
-      <c r="T4" s="189"/>
+      <c r="T4" s="184"/>
       <c r="U4" s="26" t="s">
         <v>26</v>
       </c>
@@ -22408,7 +22409,7 @@
       <c r="Z4" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="AA4" s="189"/>
+      <c r="AA4" s="184"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="76" t="s">
@@ -22483,7 +22484,7 @@
       <c r="Z5" s="79" t="s">
         <v>71</v>
       </c>
-      <c r="AA5" s="196">
+      <c r="AA5" s="185">
         <f>SUM(V5:V6,Y5:Y6)</f>
         <v>18</v>
       </c>
@@ -22553,7 +22554,7 @@
       <c r="X6" s="81"/>
       <c r="Y6" s="37"/>
       <c r="Z6" s="83"/>
-      <c r="AA6" s="184"/>
+      <c r="AA6" s="177"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
@@ -22621,7 +22622,7 @@
       <c r="Z7" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="AA7" s="184">
+      <c r="AA7" s="177">
         <f t="shared" ref="AA7" si="7">SUM(V7:V8,Y7:Y8)</f>
         <v>18</v>
       </c>
@@ -22677,7 +22678,7 @@
       <c r="Z8" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="AA8" s="184"/>
+      <c r="AA8" s="177"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="80" t="s">
@@ -22738,7 +22739,7 @@
       <c r="Z9" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="AA9" s="184">
+      <c r="AA9" s="177">
         <f t="shared" ref="AA9" si="8">SUM(V9:V10,Y9:Y10)</f>
         <v>18</v>
       </c>
@@ -22784,7 +22785,7 @@
       <c r="X10" s="81"/>
       <c r="Y10" s="37"/>
       <c r="Z10" s="83"/>
-      <c r="AA10" s="184"/>
+      <c r="AA10" s="177"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
@@ -22819,7 +22820,7 @@
       <c r="Z11" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="AA11" s="184">
+      <c r="AA11" s="177">
         <f t="shared" ref="AA11" si="9">SUM(V11:V12,Y11:Y12)</f>
         <v>18</v>
       </c>
@@ -22862,9 +22863,9 @@
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
-      <c r="O12" s="192"/>
-      <c r="P12" s="193"/>
-      <c r="Q12" s="194"/>
+      <c r="O12" s="179"/>
+      <c r="P12" s="180"/>
+      <c r="Q12" s="181"/>
       <c r="T12" s="31"/>
       <c r="U12" s="78"/>
       <c r="V12" s="33"/>
@@ -22872,7 +22873,7 @@
       <c r="X12" s="78"/>
       <c r="Y12" s="33"/>
       <c r="Z12" s="85"/>
-      <c r="AA12" s="184"/>
+      <c r="AA12" s="177"/>
     </row>
     <row r="13" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
@@ -22881,7 +22882,7 @@
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="90"/>
-      <c r="O13" s="201"/>
+      <c r="O13" s="206"/>
       <c r="P13" s="93"/>
       <c r="Q13" s="94"/>
       <c r="T13" s="47" t="s">
@@ -22905,7 +22906,7 @@
       <c r="Z13" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="AA13" s="184">
+      <c r="AA13" s="177">
         <f t="shared" ref="AA13" si="12">SUM(V13:V14,Y13:Y14)</f>
         <v>18</v>
       </c>
@@ -22927,7 +22928,7 @@
       <c r="X14" s="81"/>
       <c r="Y14" s="37"/>
       <c r="Z14" s="83"/>
-      <c r="AA14" s="184"/>
+      <c r="AA14" s="177"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="95"/>
@@ -22960,7 +22961,7 @@
       <c r="Z15" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="AA15" s="184">
+      <c r="AA15" s="177">
         <f t="shared" ref="AA15" si="13">SUM(V15:V16,Y15:Y16)</f>
         <v>18</v>
       </c>
@@ -22982,7 +22983,7 @@
       <c r="X16" s="78"/>
       <c r="Y16" s="33"/>
       <c r="Z16" s="85"/>
-      <c r="AA16" s="184"/>
+      <c r="AA16" s="177"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
@@ -23015,7 +23016,7 @@
       <c r="Z17" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="AA17" s="184">
+      <c r="AA17" s="177">
         <f t="shared" ref="AA17" si="14">SUM(V17:V18,Y17:Y18)</f>
         <v>16</v>
       </c>
@@ -23037,7 +23038,7 @@
       <c r="X18" s="96"/>
       <c r="Y18" s="65"/>
       <c r="Z18" s="98"/>
-      <c r="AA18" s="198"/>
+      <c r="AA18" s="178"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
@@ -23195,6 +23196,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AA5:AA6"/>
     <mergeCell ref="AA17:AA18"/>
     <mergeCell ref="AA9:AA10"/>
     <mergeCell ref="AA11:AA12"/>
@@ -23202,12 +23209,6 @@
     <mergeCell ref="P12:Q12"/>
     <mergeCell ref="AA13:AA14"/>
     <mergeCell ref="AA15:AA16"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AA5:AA6"/>
   </mergeCells>
   <conditionalFormatting sqref="Y20">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="notEqual">

</xml_diff>